<commit_message>
added whitebox tests to excel sheet
</commit_message>
<xml_diff>
--- a/Documents/Testing/Tests Documents/Test_case.xlsx
+++ b/Documents/Testing/Tests Documents/Test_case.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Semeter_2\SFT\Project\Project\winter24--sft221-naa-1\Documents\Testing\Tests Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/84e5bdbfc05febe3/Documents/CPASemester2/SFT221/SFT Project/winter24--sft221-naa-1/Documents/Testing/Tests Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97F81C77-F15C-4346-8ABE-44D81C23B08A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="36" documentId="13_ncr:1_{97F81C77-F15C-4346-8ABE-44D81C23B08A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3D9B390C-0D6A-4A0C-B779-7F623343FF20}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="29020" windowHeight="17500" xr2:uid="{16F36B32-E991-4A8C-AA31-131C233A1DED}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{16F36B32-E991-4A8C-AA31-131C233A1DED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="183">
   <si>
     <t>Test #</t>
   </si>
@@ -519,6 +519,72 @@
   </si>
   <si>
     <t>destination out of map</t>
+  </si>
+  <si>
+    <t>T016</t>
+  </si>
+  <si>
+    <t>WhiteBox</t>
+  </si>
+  <si>
+    <t>valid destination in input string</t>
+  </si>
+  <si>
+    <t>0 0 1A</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>Function correctly detects correct destination input</t>
+  </si>
+  <si>
+    <t>T017</t>
+  </si>
+  <si>
+    <t>T018</t>
+  </si>
+  <si>
+    <t>Whitebox</t>
+  </si>
+  <si>
+    <t>no map, null map provided</t>
+  </si>
+  <si>
+    <t>struct Map map* = NULL</t>
+  </si>
+  <si>
+    <t>Function correctly detects there is no map provided</t>
+  </si>
+  <si>
+    <t>T019</t>
+  </si>
+  <si>
+    <t>no input, null input provided</t>
+  </si>
+  <si>
+    <t>char* input = NULL</t>
+  </si>
+  <si>
+    <t>"\0"</t>
+  </si>
+  <si>
+    <t>Function correctly detects null or empty input string</t>
+  </si>
+  <si>
+    <t>exit String</t>
+  </si>
+  <si>
+    <t>char input[] = "0 0 x"</t>
+  </si>
+  <si>
+    <t>char input[] = "0 0 1A"</t>
+  </si>
+  <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t>Function corrects detects input string and returns corresponding return value</t>
   </si>
 </sst>
 </file>
@@ -677,6 +743,12 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -700,12 +772,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1041,65 +1107,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5C67FD9-2090-4A05-A979-12107FCFFDB4}">
-  <dimension ref="A1:G68"/>
+  <dimension ref="A1:G71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="D7" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="61.90625" customWidth="1"/>
-    <col min="4" max="4" width="20.453125" customWidth="1"/>
-    <col min="5" max="5" width="85.81640625" customWidth="1"/>
-    <col min="6" max="6" width="18.453125" customWidth="1"/>
-    <col min="7" max="7" width="117.453125" customWidth="1"/>
+    <col min="3" max="3" width="61.88671875" customWidth="1"/>
+    <col min="4" max="4" width="20.44140625" customWidth="1"/>
+    <col min="5" max="5" width="85.77734375" customWidth="1"/>
+    <col min="6" max="6" width="18.44140625" customWidth="1"/>
+    <col min="7" max="7" width="117.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
       <c r="G1" s="11" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="14" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="18" t="s">
+      <c r="D2" s="18"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="16"/>
+      <c r="B3" s="16"/>
       <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="4"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="21"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F3" s="21"/>
+      <c r="G3" s="13"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
@@ -1119,7 +1185,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>12</v>
       </c>
@@ -1139,7 +1205,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>16</v>
       </c>
@@ -1159,7 +1225,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>21</v>
       </c>
@@ -1179,7 +1245,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>24</v>
       </c>
@@ -1199,7 +1265,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>28</v>
       </c>
@@ -1219,7 +1285,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>29</v>
       </c>
@@ -1239,7 +1305,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>30</v>
       </c>
@@ -1259,7 +1325,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>32</v>
       </c>
@@ -1279,28 +1345,28 @@
         <v>159</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="G13" s="7"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D14" s="10"/>
       <c r="G14" s="7"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="12" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
       <c r="G15" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -1317,13 +1383,13 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
         <v>5</v>
       </c>
       <c r="G17" s="7"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>36</v>
       </c>
@@ -1343,7 +1409,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>40</v>
       </c>
@@ -1363,7 +1429,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>43</v>
       </c>
@@ -1383,7 +1449,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>47</v>
       </c>
@@ -1403,7 +1469,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>51</v>
       </c>
@@ -1423,7 +1489,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>55</v>
       </c>
@@ -1443,151 +1509,171 @@
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="G24" s="7"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A25" s="12" t="s">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>161</v>
+      </c>
+      <c r="B24" t="s">
+        <v>169</v>
+      </c>
+      <c r="C24" t="s">
+        <v>174</v>
+      </c>
+      <c r="D24" t="s">
+        <v>175</v>
+      </c>
+      <c r="E24" t="s">
+        <v>176</v>
+      </c>
+      <c r="F24" t="s">
+        <v>165</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>167</v>
+      </c>
+      <c r="B25" t="s">
+        <v>169</v>
+      </c>
+      <c r="C25" t="s">
+        <v>178</v>
+      </c>
+      <c r="D25" t="s">
+        <v>179</v>
+      </c>
+      <c r="E25" t="s">
+        <v>38</v>
+      </c>
+      <c r="F25" t="s">
+        <v>165</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>168</v>
+      </c>
+      <c r="B26" t="s">
+        <v>169</v>
+      </c>
+      <c r="C26" t="s">
+        <v>170</v>
+      </c>
+      <c r="D26" t="s">
+        <v>171</v>
+      </c>
+      <c r="E26" t="s">
+        <v>181</v>
+      </c>
+      <c r="F26" t="s">
+        <v>165</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>173</v>
+      </c>
+      <c r="B27" t="s">
+        <v>162</v>
+      </c>
+      <c r="C27" t="s">
+        <v>163</v>
+      </c>
+      <c r="D27" t="s">
+        <v>180</v>
+      </c>
+      <c r="E27" t="s">
+        <v>164</v>
+      </c>
+      <c r="F27" t="s">
+        <v>165</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="B25" s="13"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="1" t="s">
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>0</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B29" t="s">
         <v>1</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C29" t="s">
         <v>2</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F29" t="s">
         <v>3</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G29" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C27" t="s">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C30" t="s">
         <v>61</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D30" t="s">
         <v>62</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E30" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>102</v>
       </c>
-      <c r="B28" t="s">
-        <v>7</v>
-      </c>
-      <c r="C28">
+      <c r="B31" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31">
         <v>1</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D31" t="s">
         <v>64</v>
-      </c>
-      <c r="E28">
-        <v>3</v>
-      </c>
-      <c r="F28" t="s">
-        <v>10</v>
-      </c>
-      <c r="G28" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>103</v>
-      </c>
-      <c r="B29" t="s">
-        <v>7</v>
-      </c>
-      <c r="C29">
-        <v>7</v>
-      </c>
-      <c r="D29" t="s">
-        <v>66</v>
-      </c>
-      <c r="E29">
-        <v>3</v>
-      </c>
-      <c r="F29" t="s">
-        <v>19</v>
-      </c>
-      <c r="G29" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>104</v>
-      </c>
-      <c r="B30" t="s">
-        <v>7</v>
-      </c>
-      <c r="C30" t="s">
-        <v>68</v>
-      </c>
-      <c r="D30" t="s">
-        <v>66</v>
-      </c>
-      <c r="E30">
-        <v>3</v>
-      </c>
-      <c r="F30" t="s">
-        <v>19</v>
-      </c>
-      <c r="G30" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>105</v>
-      </c>
-      <c r="B31" t="s">
-        <v>7</v>
-      </c>
-      <c r="C31" t="s">
-        <v>70</v>
-      </c>
-      <c r="D31" t="s">
-        <v>66</v>
       </c>
       <c r="E31">
         <v>3</v>
       </c>
       <c r="F31" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G31" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B32" t="s">
         <v>7</v>
       </c>
-      <c r="C32" t="s">
-        <v>72</v>
+      <c r="C32">
+        <v>7</v>
       </c>
       <c r="D32" t="s">
         <v>66</v>
@@ -1599,498 +1685,568 @@
         <v>19</v>
       </c>
       <c r="G32" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>104</v>
+      </c>
+      <c r="B33" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" t="s">
+        <v>68</v>
+      </c>
+      <c r="D33" t="s">
+        <v>66</v>
+      </c>
+      <c r="E33">
+        <v>3</v>
+      </c>
+      <c r="F33" t="s">
+        <v>19</v>
+      </c>
+      <c r="G33" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>105</v>
+      </c>
+      <c r="B34" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" t="s">
+        <v>70</v>
+      </c>
+      <c r="D34" t="s">
+        <v>66</v>
+      </c>
+      <c r="E34">
+        <v>3</v>
+      </c>
+      <c r="F34" t="s">
+        <v>19</v>
+      </c>
+      <c r="G34" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>106</v>
+      </c>
+      <c r="B35" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" t="s">
+        <v>72</v>
+      </c>
+      <c r="D35" t="s">
+        <v>66</v>
+      </c>
+      <c r="E35">
+        <v>3</v>
+      </c>
+      <c r="F35" t="s">
+        <v>19</v>
+      </c>
+      <c r="G35" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A34" s="12" t="s">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="B34" s="13"/>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="1" t="s">
+      <c r="B37" s="15"/>
+      <c r="C37" s="15"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
         <v>0</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B38" t="s">
         <v>1</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C38" t="s">
         <v>2</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D38" t="s">
         <v>3</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E38" t="s">
         <v>4</v>
       </c>
-      <c r="F35" t="s">
+      <c r="F38" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
         <v>76</v>
       </c>
-      <c r="B36" t="s">
-        <v>7</v>
-      </c>
-      <c r="C36" t="s">
+      <c r="B39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C39" t="s">
         <v>77</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D39" t="s">
         <v>10</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E39" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
         <v>79</v>
       </c>
-      <c r="B37" t="s">
-        <v>7</v>
-      </c>
-      <c r="C37" t="s">
+      <c r="B40" t="s">
+        <v>7</v>
+      </c>
+      <c r="C40" t="s">
         <v>151</v>
-      </c>
-      <c r="D37" t="s">
-        <v>10</v>
-      </c>
-      <c r="E37" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>81</v>
-      </c>
-      <c r="B38" t="s">
-        <v>7</v>
-      </c>
-      <c r="C38" t="s">
-        <v>152</v>
-      </c>
-      <c r="D38" t="s">
-        <v>19</v>
-      </c>
-      <c r="E38" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>83</v>
-      </c>
-      <c r="B39" t="s">
-        <v>7</v>
-      </c>
-      <c r="C39" t="s">
-        <v>84</v>
-      </c>
-      <c r="D39" t="s">
-        <v>19</v>
-      </c>
-      <c r="E39" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>86</v>
-      </c>
-      <c r="B40" t="s">
-        <v>7</v>
-      </c>
-      <c r="C40" t="s">
-        <v>87</v>
       </c>
       <c r="D40" t="s">
         <v>10</v>
       </c>
       <c r="E40" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="B41" t="s">
         <v>7</v>
       </c>
       <c r="C41" t="s">
-        <v>90</v>
+        <v>152</v>
       </c>
       <c r="D41" t="s">
         <v>19</v>
       </c>
       <c r="E41" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>83</v>
+      </c>
+      <c r="B42" t="s">
+        <v>7</v>
+      </c>
+      <c r="C42" t="s">
+        <v>84</v>
+      </c>
+      <c r="D42" t="s">
+        <v>19</v>
+      </c>
+      <c r="E42" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>86</v>
+      </c>
+      <c r="B43" t="s">
+        <v>7</v>
+      </c>
+      <c r="C43" t="s">
+        <v>87</v>
+      </c>
+      <c r="D43" t="s">
+        <v>10</v>
+      </c>
+      <c r="E43" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>89</v>
+      </c>
+      <c r="B44" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44" t="s">
+        <v>90</v>
+      </c>
+      <c r="D44" t="s">
+        <v>19</v>
+      </c>
+      <c r="E44" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A43" s="12" t="s">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="B43" s="13"/>
-      <c r="C43" s="13"/>
-      <c r="D43" s="13"/>
-      <c r="E43" s="13"/>
-      <c r="F43" s="13"/>
-      <c r="G43" s="1" t="s">
+      <c r="B46" s="15"/>
+      <c r="C46" s="15"/>
+      <c r="D46" s="15"/>
+      <c r="E46" s="15"/>
+      <c r="F46" s="15"/>
+      <c r="G46" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
         <v>0</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B47" t="s">
         <v>1</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C47" t="s">
         <v>2</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D47" t="s">
         <v>3</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E47" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C45" t="s">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C48" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
         <v>107</v>
       </c>
-      <c r="B46" t="s">
-        <v>7</v>
-      </c>
-      <c r="C46" t="s">
+      <c r="B49" t="s">
+        <v>7</v>
+      </c>
+      <c r="C49" t="s">
         <v>93</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D49" t="s">
         <v>10</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E49" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
         <v>108</v>
       </c>
-      <c r="B47" t="s">
-        <v>7</v>
-      </c>
-      <c r="C47" t="s">
+      <c r="B50" t="s">
+        <v>7</v>
+      </c>
+      <c r="C50" t="s">
         <v>95</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D50" t="s">
         <v>96</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E50" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
         <v>109</v>
       </c>
-      <c r="B48" t="s">
-        <v>7</v>
-      </c>
-      <c r="C48" t="s">
+      <c r="B51" t="s">
+        <v>7</v>
+      </c>
+      <c r="C51" t="s">
         <v>98</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D51" t="s">
         <v>96</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E51" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
         <v>110</v>
       </c>
-      <c r="B49" t="s">
-        <v>7</v>
-      </c>
-      <c r="C49" t="s">
+      <c r="B52" t="s">
+        <v>7</v>
+      </c>
+      <c r="C52" t="s">
         <v>100</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D52" t="s">
         <v>96</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E52" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A52" s="12" t="s">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A55" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="B52" s="13"/>
-      <c r="C52" s="13"/>
-      <c r="D52" s="13"/>
-      <c r="E52" s="13"/>
-      <c r="F52" s="13"/>
-      <c r="G52" s="1" t="s">
+      <c r="B55" s="15"/>
+      <c r="C55" s="15"/>
+      <c r="D55" s="15"/>
+      <c r="E55" s="15"/>
+      <c r="F55" s="15"/>
+      <c r="G55" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
         <v>0</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B56" t="s">
         <v>1</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C56" t="s">
         <v>2</v>
       </c>
-      <c r="F53" t="s">
+      <c r="F56" t="s">
         <v>3</v>
       </c>
-      <c r="G53" t="s">
+      <c r="G56" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
         <v>111</v>
       </c>
-      <c r="B55" t="s">
-        <v>7</v>
-      </c>
-      <c r="C55" t="s">
+      <c r="B58" t="s">
+        <v>7</v>
+      </c>
+      <c r="C58" t="s">
         <v>112</v>
-      </c>
-      <c r="F55" t="s">
-        <v>113</v>
-      </c>
-      <c r="G55" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
-        <v>115</v>
-      </c>
-      <c r="B56" t="s">
-        <v>7</v>
-      </c>
-      <c r="C56" t="s">
-        <v>116</v>
-      </c>
-      <c r="F56" t="s">
-        <v>113</v>
-      </c>
-      <c r="G56" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
-        <v>118</v>
-      </c>
-      <c r="B57" t="s">
-        <v>7</v>
-      </c>
-      <c r="C57" t="s">
-        <v>119</v>
-      </c>
-      <c r="F57" t="s">
-        <v>113</v>
-      </c>
-      <c r="G57" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A58" t="s">
-        <v>121</v>
-      </c>
-      <c r="B58" t="s">
-        <v>7</v>
-      </c>
-      <c r="C58" t="s">
-        <v>18</v>
       </c>
       <c r="F58" t="s">
         <v>113</v>
       </c>
       <c r="G58" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>115</v>
+      </c>
+      <c r="B59" t="s">
+        <v>7</v>
+      </c>
+      <c r="C59" t="s">
+        <v>116</v>
+      </c>
+      <c r="F59" t="s">
+        <v>113</v>
+      </c>
+      <c r="G59" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>118</v>
+      </c>
+      <c r="B60" t="s">
+        <v>7</v>
+      </c>
+      <c r="C60" t="s">
+        <v>119</v>
+      </c>
+      <c r="F60" t="s">
+        <v>113</v>
+      </c>
+      <c r="G60" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>121</v>
+      </c>
+      <c r="B61" t="s">
+        <v>7</v>
+      </c>
+      <c r="C61" t="s">
+        <v>18</v>
+      </c>
+      <c r="F61" t="s">
+        <v>113</v>
+      </c>
+      <c r="G61" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
         <v>123</v>
       </c>
-      <c r="B59" t="s">
-        <v>7</v>
-      </c>
-      <c r="C59" t="s">
+      <c r="B62" t="s">
+        <v>7</v>
+      </c>
+      <c r="C62" t="s">
         <v>124</v>
       </c>
-      <c r="F59" t="s">
+      <c r="F62" t="s">
         <v>10</v>
       </c>
-      <c r="G59" t="s">
+      <c r="G62" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A61" s="12" t="s">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A64" s="14" t="s">
         <v>150</v>
       </c>
-      <c r="B61" s="13"/>
-      <c r="C61" s="13"/>
-      <c r="D61" s="13"/>
-      <c r="E61" s="13"/>
-      <c r="F61" s="13"/>
-      <c r="G61" s="1" t="s">
+      <c r="B64" s="15"/>
+      <c r="C64" s="15"/>
+      <c r="D64" s="15"/>
+      <c r="E64" s="15"/>
+      <c r="F64" s="15"/>
+      <c r="G64" s="1" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A62" t="s">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
         <v>0</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B65" t="s">
         <v>1</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C65" t="s">
         <v>2</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D65" t="s">
         <v>127</v>
       </c>
-      <c r="E62" t="s">
+      <c r="E65" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C63" t="s">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C66" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A64" t="s">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
         <v>141</v>
       </c>
-      <c r="B64" t="s">
-        <v>7</v>
-      </c>
-      <c r="C64" t="s">
+      <c r="B67" t="s">
+        <v>7</v>
+      </c>
+      <c r="C67" t="s">
         <v>129</v>
-      </c>
-      <c r="D64" t="s">
-        <v>130</v>
-      </c>
-      <c r="E64" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A65" t="s">
-        <v>142</v>
-      </c>
-      <c r="B65" t="s">
-        <v>7</v>
-      </c>
-      <c r="C65" t="s">
-        <v>132</v>
-      </c>
-      <c r="D65">
-        <v>6.7</v>
-      </c>
-      <c r="E65" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A66" t="s">
-        <v>143</v>
-      </c>
-      <c r="B66" t="s">
-        <v>7</v>
-      </c>
-      <c r="C66" t="s">
-        <v>134</v>
-      </c>
-      <c r="D66">
-        <v>0</v>
-      </c>
-      <c r="E66" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A67" t="s">
-        <v>144</v>
-      </c>
-      <c r="B67" t="s">
-        <v>7</v>
-      </c>
-      <c r="C67" t="s">
-        <v>136</v>
       </c>
       <c r="D67" t="s">
         <v>130</v>
       </c>
       <c r="E67" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>142</v>
+      </c>
+      <c r="B68" t="s">
+        <v>7</v>
+      </c>
+      <c r="C68" t="s">
+        <v>132</v>
+      </c>
+      <c r="D68">
+        <v>6.7</v>
+      </c>
+      <c r="E68" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>143</v>
+      </c>
+      <c r="B69" t="s">
+        <v>7</v>
+      </c>
+      <c r="C69" t="s">
+        <v>134</v>
+      </c>
+      <c r="D69">
+        <v>0</v>
+      </c>
+      <c r="E69" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>144</v>
+      </c>
+      <c r="B70" t="s">
+        <v>7</v>
+      </c>
+      <c r="C70" t="s">
+        <v>136</v>
+      </c>
+      <c r="D70" t="s">
+        <v>130</v>
+      </c>
+      <c r="E70" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A68" t="s">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
         <v>145</v>
       </c>
-      <c r="B68" t="s">
-        <v>7</v>
-      </c>
-      <c r="C68" t="s">
+      <c r="B71" t="s">
+        <v>7</v>
+      </c>
+      <c r="C71" t="s">
         <v>138</v>
       </c>
-      <c r="D68">
+      <c r="D71">
         <v>35.35</v>
       </c>
-      <c r="E68" t="s">
+      <c r="E71" t="s">
         <v>139</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="A34:F34"/>
-    <mergeCell ref="A43:F43"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="A61:F61"/>
-    <mergeCell ref="A15:F15"/>
-    <mergeCell ref="A25:F25"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="A37:F37"/>
+    <mergeCell ref="A46:F46"/>
+    <mergeCell ref="A55:F55"/>
+    <mergeCell ref="A64:F64"/>
+    <mergeCell ref="A15:F15"/>
+    <mergeCell ref="A28:F28"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added tests for check weight whitebox
</commit_message>
<xml_diff>
--- a/Documents/Testing/Tests Documents/Test_case.xlsx
+++ b/Documents/Testing/Tests Documents/Test_case.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f6642f03d3f68a2f/Desktop/New folder (3)/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sft project\winter24--sft221-naa-1\Documents\Testing\Tests Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="13_ncr:1_{2346BDC1-5429-4EF5-832C-DA8CE3F4108A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0058F2BD-99CF-43D2-B0AA-2F352E6A04EE}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7782F872-E008-4F0E-864F-C667BC6D9785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{16F36B32-E991-4A8C-AA31-131C233A1DED}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="201">
   <si>
     <t>Test #</t>
   </si>
@@ -255,9 +255,6 @@
     <t>FUNCTION: CheckWeight</t>
   </si>
   <si>
-    <t>l</t>
-  </si>
-  <si>
     <t>T021</t>
   </si>
   <si>
@@ -598,6 +595,48 @@
   </si>
   <si>
     <t>1 fail result returned 0</t>
+  </si>
+  <si>
+    <t>T027</t>
+  </si>
+  <si>
+    <t>Whitebox</t>
+  </si>
+  <si>
+    <t>The truck can carry an additional package when it's already near its weight capacity.</t>
+  </si>
+  <si>
+    <t>T028</t>
+  </si>
+  <si>
+    <t>Truck weight = 1000.5 kg, New weight = 199.4 kg</t>
+  </si>
+  <si>
+    <t>Function handles floating-point weights summing close to but not over the weight limit.</t>
+  </si>
+  <si>
+    <t>T029</t>
+  </si>
+  <si>
+    <t>Truck weight = 1000.6 kg, New weight = 199.5 kg</t>
+  </si>
+  <si>
+    <t>T030</t>
+  </si>
+  <si>
+    <t>Truck weight = 1200 kg, New weight = 1 kg</t>
+  </si>
+  <si>
+    <t>Tes+A51+A60:G66</t>
+  </si>
+  <si>
+    <t>Truck weight = 1199 kg, New weight = 1 kg</t>
+  </si>
+  <si>
+    <t>Checks precission with floating-point numbers resulting in total just over the weight limit.</t>
+  </si>
+  <si>
+    <t>A full truck cannot take on even the smallest valid package weight or not</t>
   </si>
 </sst>
 </file>
@@ -756,6 +795,12 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -779,12 +824,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1120,10 +1159,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5C67FD9-2090-4A05-A979-12107FCFFDB4}">
-  <dimension ref="A1:G72"/>
+  <dimension ref="A1:G75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B43" workbookViewId="0">
-      <selection activeCell="E54" sqref="E54"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1136,47 +1175,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
       <c r="G1" s="11" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="18" t="s">
+      <c r="D2" s="18"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="12" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
+      <c r="A3" s="16"/>
+      <c r="B3" s="16"/>
       <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="4"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="13"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
@@ -1283,7 +1322,7 @@
         <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>25</v>
@@ -1303,19 +1342,19 @@
         <v>29</v>
       </c>
       <c r="B10" t="s">
+        <v>145</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>146</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>147</v>
       </c>
       <c r="F10" t="s">
         <v>19</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -1323,7 +1362,7 @@
         <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>31</v>
@@ -1335,7 +1374,7 @@
         <v>19</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -1343,19 +1382,19 @@
         <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>31</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F12" t="s">
         <v>19</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -1367,14 +1406,14 @@
       <c r="G14" s="7"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
       <c r="G15" s="1" t="s">
         <v>35</v>
       </c>
@@ -1404,94 +1443,94 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B18" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C18" t="s">
+        <v>162</v>
+      </c>
+      <c r="D18" t="s">
         <v>163</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>164</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
+        <v>154</v>
+      </c>
+      <c r="G18" s="7" t="s">
         <v>165</v>
-      </c>
-      <c r="F18" t="s">
-        <v>155</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B19" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C19" t="s">
+        <v>166</v>
+      </c>
+      <c r="D19" t="s">
         <v>167</v>
-      </c>
-      <c r="D19" t="s">
-        <v>168</v>
       </c>
       <c r="E19" t="s">
         <v>37</v>
       </c>
       <c r="F19" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>157</v>
+      </c>
+      <c r="B20" t="s">
+        <v>171</v>
+      </c>
+      <c r="C20" t="s">
         <v>158</v>
       </c>
-      <c r="B20" t="s">
-        <v>172</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>159</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
+        <v>169</v>
+      </c>
+      <c r="F20" t="s">
+        <v>154</v>
+      </c>
+      <c r="G20" s="7" t="s">
         <v>160</v>
-      </c>
-      <c r="E20" t="s">
-        <v>170</v>
-      </c>
-      <c r="F20" t="s">
-        <v>155</v>
-      </c>
-      <c r="G20" s="7" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B21" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C21" t="s">
+        <v>152</v>
+      </c>
+      <c r="D21" t="s">
+        <v>168</v>
+      </c>
+      <c r="E21" t="s">
         <v>153</v>
       </c>
-      <c r="D21" t="s">
-        <v>169</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>154</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" s="7" t="s">
         <v>155</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
@@ -1499,7 +1538,7 @@
         <v>38</v>
       </c>
       <c r="B22" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C22" t="s">
         <v>36</v>
@@ -1519,7 +1558,7 @@
         <v>41</v>
       </c>
       <c r="B23" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C23" t="s">
         <v>42</v>
@@ -1539,7 +1578,7 @@
         <v>45</v>
       </c>
       <c r="B24" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C24" t="s">
         <v>46</v>
@@ -1559,7 +1598,7 @@
         <v>49</v>
       </c>
       <c r="B25" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C25" t="s">
         <v>50</v>
@@ -1579,7 +1618,7 @@
         <v>53</v>
       </c>
       <c r="B26" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C26" t="s">
         <v>54</v>
@@ -1595,14 +1634,14 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="B27" s="13"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
+      <c r="A27" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
       <c r="G27" s="1" t="s">
         <v>58</v>
       </c>
@@ -1637,7 +1676,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B30" t="s">
         <v>7</v>
@@ -1660,7 +1699,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B31" t="s">
         <v>7</v>
@@ -1683,7 +1722,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B32" t="s">
         <v>7</v>
@@ -1706,7 +1745,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B33" t="s">
         <v>7</v>
@@ -1729,7 +1768,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B34" t="s">
         <v>7</v>
@@ -1751,14 +1790,14 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="B36" s="13"/>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
+      <c r="A36" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="B36" s="15"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="15"/>
+      <c r="F36" s="15"/>
       <c r="G36" s="1" t="s">
         <v>72</v>
       </c>
@@ -1779,515 +1818,580 @@
       <c r="E37" t="s">
         <v>4</v>
       </c>
-      <c r="F37" t="s">
-        <v>73</v>
-      </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
+        <v>73</v>
+      </c>
+      <c r="B38" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" t="s">
         <v>74</v>
-      </c>
-      <c r="B38" t="s">
-        <v>7</v>
-      </c>
-      <c r="C38" t="s">
-        <v>75</v>
       </c>
       <c r="D38" t="s">
         <v>10</v>
       </c>
       <c r="E38" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B39" t="s">
         <v>7</v>
       </c>
       <c r="C39" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D39" t="s">
         <v>10</v>
       </c>
       <c r="E39" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B40" t="s">
         <v>7</v>
       </c>
       <c r="C40" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D40" t="s">
         <v>19</v>
       </c>
       <c r="E40" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
+        <v>80</v>
+      </c>
+      <c r="B41" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41" t="s">
         <v>81</v>
-      </c>
-      <c r="B41" t="s">
-        <v>7</v>
-      </c>
-      <c r="C41" t="s">
-        <v>82</v>
       </c>
       <c r="D41" t="s">
         <v>19</v>
       </c>
       <c r="E41" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
+        <v>83</v>
+      </c>
+      <c r="B42" t="s">
+        <v>7</v>
+      </c>
+      <c r="C42" t="s">
         <v>84</v>
-      </c>
-      <c r="B42" t="s">
-        <v>7</v>
-      </c>
-      <c r="C42" t="s">
-        <v>85</v>
       </c>
       <c r="D42" t="s">
         <v>10</v>
       </c>
       <c r="E42" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
+        <v>86</v>
+      </c>
+      <c r="B43" t="s">
+        <v>7</v>
+      </c>
+      <c r="C43" t="s">
         <v>87</v>
-      </c>
-      <c r="B43" t="s">
-        <v>7</v>
-      </c>
-      <c r="C43" t="s">
-        <v>88</v>
       </c>
       <c r="D43" t="s">
         <v>19</v>
       </c>
       <c r="E43" t="s">
-        <v>89</v>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>187</v>
+      </c>
+      <c r="B44" t="s">
+        <v>188</v>
+      </c>
+      <c r="C44" t="s">
+        <v>198</v>
+      </c>
+      <c r="D44" t="s">
+        <v>10</v>
+      </c>
+      <c r="E44" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="B45" s="13"/>
-      <c r="C45" s="13"/>
-      <c r="D45" s="13"/>
-      <c r="E45" s="13"/>
-      <c r="F45" s="13"/>
-      <c r="G45" s="1" t="s">
-        <v>90</v>
+      <c r="A45" t="s">
+        <v>190</v>
+      </c>
+      <c r="B45" t="s">
+        <v>188</v>
+      </c>
+      <c r="C45" t="s">
+        <v>191</v>
+      </c>
+      <c r="D45" t="s">
+        <v>10</v>
+      </c>
+      <c r="E45" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>0</v>
+        <v>193</v>
       </c>
       <c r="B46" t="s">
-        <v>1</v>
+        <v>188</v>
       </c>
       <c r="C46" t="s">
-        <v>2</v>
+        <v>194</v>
       </c>
       <c r="D46" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="E46" t="s">
-        <v>4</v>
+        <v>199</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>195</v>
+      </c>
+      <c r="B47" t="s">
+        <v>188</v>
+      </c>
       <c r="C47" t="s">
-        <v>59</v>
+        <v>196</v>
+      </c>
+      <c r="D47" t="s">
+        <v>19</v>
+      </c>
+      <c r="E47" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>100</v>
-      </c>
-      <c r="B48" t="s">
-        <v>7</v>
-      </c>
-      <c r="C48" t="s">
-        <v>174</v>
-      </c>
-      <c r="D48" t="s">
-        <v>92</v>
-      </c>
-      <c r="E48" t="s">
-        <v>91</v>
+      <c r="A48" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="B48" s="15"/>
+      <c r="C48" s="15"/>
+      <c r="D48" s="15"/>
+      <c r="E48" s="15"/>
+      <c r="F48" s="15"/>
+      <c r="G48" s="1" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>101</v>
+        <v>0</v>
       </c>
       <c r="B49" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C49" t="s">
-        <v>175</v>
+        <v>2</v>
       </c>
       <c r="D49" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E49" t="s">
-        <v>93</v>
+        <v>4</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>102</v>
-      </c>
-      <c r="B50" t="s">
-        <v>7</v>
-      </c>
       <c r="C50" t="s">
-        <v>176</v>
-      </c>
-      <c r="D50" t="s">
-        <v>92</v>
-      </c>
-      <c r="E50" t="s">
-        <v>94</v>
+        <v>59</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B51" t="s">
         <v>7</v>
       </c>
       <c r="C51" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="D51" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E51" t="s">
-        <v>184</v>
+        <v>90</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>178</v>
+        <v>100</v>
       </c>
       <c r="B52" t="s">
-        <v>173</v>
+        <v>7</v>
       </c>
       <c r="C52" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="D52" t="s">
-        <v>155</v>
+        <v>10</v>
       </c>
       <c r="E52" t="s">
-        <v>185</v>
+        <v>92</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>179</v>
+        <v>101</v>
       </c>
       <c r="B53" t="s">
-        <v>173</v>
+        <v>7</v>
       </c>
       <c r="C53" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="D53" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E53" t="s">
-        <v>186</v>
+        <v>93</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
+        <v>102</v>
+      </c>
+      <c r="B54" t="s">
+        <v>7</v>
+      </c>
+      <c r="C54" t="s">
+        <v>176</v>
+      </c>
+      <c r="D54" t="s">
+        <v>91</v>
+      </c>
+      <c r="E54" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>177</v>
+      </c>
+      <c r="B55" t="s">
+        <v>172</v>
+      </c>
+      <c r="C55" t="s">
         <v>180</v>
       </c>
-      <c r="B54" t="s">
-        <v>173</v>
-      </c>
-      <c r="C54" t="s">
-        <v>183</v>
-      </c>
-      <c r="D54" t="s">
-        <v>92</v>
-      </c>
-      <c r="E54" t="s">
-        <v>187</v>
+      <c r="D55" t="s">
+        <v>154</v>
+      </c>
+      <c r="E55" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A56" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="B56" s="13"/>
-      <c r="C56" s="13"/>
-      <c r="D56" s="13"/>
-      <c r="E56" s="13"/>
-      <c r="F56" s="13"/>
-      <c r="G56" s="1" t="s">
-        <v>119</v>
+      <c r="A56" t="s">
+        <v>178</v>
+      </c>
+      <c r="B56" t="s">
+        <v>172</v>
+      </c>
+      <c r="C56" t="s">
+        <v>181</v>
+      </c>
+      <c r="D56" t="s">
+        <v>91</v>
+      </c>
+      <c r="E56" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>0</v>
+        <v>179</v>
       </c>
       <c r="B57" t="s">
-        <v>1</v>
+        <v>172</v>
       </c>
       <c r="C57" t="s">
-        <v>2</v>
-      </c>
-      <c r="F57" t="s">
-        <v>3</v>
-      </c>
-      <c r="G57" t="s">
-        <v>4</v>
+        <v>182</v>
+      </c>
+      <c r="D57" t="s">
+        <v>91</v>
+      </c>
+      <c r="E57" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
-        <v>104</v>
-      </c>
-      <c r="B59" t="s">
-        <v>7</v>
-      </c>
-      <c r="C59" t="s">
-        <v>105</v>
-      </c>
-      <c r="F59" t="s">
-        <v>106</v>
-      </c>
-      <c r="G59" t="s">
-        <v>107</v>
+      <c r="A59" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="B59" s="15"/>
+      <c r="C59" s="15"/>
+      <c r="D59" s="15"/>
+      <c r="E59" s="15"/>
+      <c r="F59" s="15"/>
+      <c r="G59" s="1" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>108</v>
+        <v>197</v>
       </c>
       <c r="B60" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C60" t="s">
-        <v>109</v>
+        <v>2</v>
       </c>
       <c r="F60" t="s">
-        <v>106</v>
+        <v>3</v>
       </c>
       <c r="G60" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
-        <v>111</v>
-      </c>
-      <c r="B61" t="s">
-        <v>7</v>
-      </c>
-      <c r="C61" t="s">
-        <v>112</v>
-      </c>
-      <c r="F61" t="s">
-        <v>106</v>
-      </c>
-      <c r="G61" t="s">
-        <v>113</v>
+        <v>4</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="B62" t="s">
         <v>7</v>
       </c>
       <c r="C62" t="s">
-        <v>18</v>
+        <v>104</v>
       </c>
       <c r="F62" t="s">
+        <v>105</v>
+      </c>
+      <c r="G62" t="s">
         <v>106</v>
-      </c>
-      <c r="G62" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="B63" t="s">
         <v>7</v>
       </c>
       <c r="C63" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="F63" t="s">
-        <v>10</v>
+        <v>105</v>
       </c>
       <c r="G63" t="s">
-        <v>118</v>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>110</v>
+      </c>
+      <c r="B64" t="s">
+        <v>7</v>
+      </c>
+      <c r="C64" t="s">
+        <v>111</v>
+      </c>
+      <c r="F64" t="s">
+        <v>105</v>
+      </c>
+      <c r="G64" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A65" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="B65" s="13"/>
-      <c r="C65" s="13"/>
-      <c r="D65" s="13"/>
-      <c r="E65" s="13"/>
-      <c r="F65" s="13"/>
-      <c r="G65" s="1" t="s">
-        <v>133</v>
+      <c r="A65" t="s">
+        <v>113</v>
+      </c>
+      <c r="B65" t="s">
+        <v>7</v>
+      </c>
+      <c r="C65" t="s">
+        <v>18</v>
+      </c>
+      <c r="F65" t="s">
+        <v>105</v>
+      </c>
+      <c r="G65" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>0</v>
+        <v>115</v>
       </c>
       <c r="B66" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C66" t="s">
-        <v>2</v>
-      </c>
-      <c r="D66" t="s">
-        <v>120</v>
-      </c>
-      <c r="E66" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C67" t="s">
-        <v>121</v>
+        <v>116</v>
+      </c>
+      <c r="F66" t="s">
+        <v>10</v>
+      </c>
+      <c r="G66" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
-        <v>134</v>
-      </c>
-      <c r="B68" t="s">
-        <v>7</v>
-      </c>
-      <c r="C68" t="s">
-        <v>122</v>
-      </c>
-      <c r="D68" t="s">
-        <v>123</v>
-      </c>
-      <c r="E68" t="s">
-        <v>124</v>
+      <c r="A68" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="B68" s="15"/>
+      <c r="C68" s="15"/>
+      <c r="D68" s="15"/>
+      <c r="E68" s="15"/>
+      <c r="F68" s="15"/>
+      <c r="G68" s="1" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>135</v>
+        <v>0</v>
       </c>
       <c r="B69" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C69" t="s">
-        <v>125</v>
-      </c>
-      <c r="D69">
-        <v>6.7</v>
+        <v>2</v>
+      </c>
+      <c r="D69" t="s">
+        <v>119</v>
       </c>
       <c r="E69" t="s">
-        <v>126</v>
+        <v>4</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
-        <v>136</v>
-      </c>
-      <c r="B70" t="s">
-        <v>7</v>
-      </c>
       <c r="C70" t="s">
-        <v>127</v>
-      </c>
-      <c r="D70">
-        <v>0</v>
-      </c>
-      <c r="E70" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B71" t="s">
         <v>7</v>
       </c>
       <c r="C71" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="D71" t="s">
+        <v>122</v>
+      </c>
+      <c r="E71" t="s">
         <v>123</v>
-      </c>
-      <c r="E71" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B72" t="s">
         <v>7</v>
       </c>
       <c r="C72" t="s">
+        <v>124</v>
+      </c>
+      <c r="D72">
+        <v>6.7</v>
+      </c>
+      <c r="E72" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>135</v>
+      </c>
+      <c r="B73" t="s">
+        <v>7</v>
+      </c>
+      <c r="C73" t="s">
+        <v>126</v>
+      </c>
+      <c r="D73">
+        <v>0</v>
+      </c>
+      <c r="E73" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>136</v>
+      </c>
+      <c r="B74" t="s">
+        <v>7</v>
+      </c>
+      <c r="C74" t="s">
+        <v>128</v>
+      </c>
+      <c r="D74" t="s">
+        <v>122</v>
+      </c>
+      <c r="E74" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>137</v>
+      </c>
+      <c r="B75" t="s">
+        <v>7</v>
+      </c>
+      <c r="C75" t="s">
+        <v>130</v>
+      </c>
+      <c r="D75">
+        <v>35.35</v>
+      </c>
+      <c r="E75" t="s">
         <v>131</v>
-      </c>
-      <c r="D72">
-        <v>35.35</v>
-      </c>
-      <c r="E72" t="s">
-        <v>132</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="A36:F36"/>
-    <mergeCell ref="A45:F45"/>
-    <mergeCell ref="A56:F56"/>
-    <mergeCell ref="A65:F65"/>
-    <mergeCell ref="A15:F15"/>
-    <mergeCell ref="A27:F27"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="A36:F36"/>
+    <mergeCell ref="A48:F48"/>
+    <mergeCell ref="A59:F59"/>
+    <mergeCell ref="A68:F68"/>
+    <mergeCell ref="A15:F15"/>
+    <mergeCell ref="A27:F27"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added white box test cases for checkboxsize
</commit_message>
<xml_diff>
--- a/Documents/Testing/Tests Documents/Test_case.xlsx
+++ b/Documents/Testing/Tests Documents/Test_case.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sft project\winter24--sft221-naa-1\Documents\Testing\Tests Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jashandeep/Documents/GitHub/winter24--sft221-naa-1/Documents/Testing/Tests Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7782F872-E008-4F0E-864F-C667BC6D9785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69328244-2CD2-EA41-8655-514E03C893D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{16F36B32-E991-4A8C-AA31-131C233A1DED}"/>
+    <workbookView xWindow="0" yWindow="640" windowWidth="29020" windowHeight="17100" xr2:uid="{16F36B32-E991-4A8C-AA31-131C233A1DED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,6 +27,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="187">
   <si>
     <t>Test #</t>
   </si>
@@ -255,6 +257,9 @@
     <t>FUNCTION: CheckWeight</t>
   </si>
   <si>
+    <t>l</t>
+  </si>
+  <si>
     <t>T021</t>
   </si>
   <si>
@@ -306,15 +311,30 @@
     <t>FUNCTION: checkspaceoftruck</t>
   </si>
   <si>
+    <t xml:space="preserve">length=5, width=3, height=2, availableLength=8, availableWidth=8, availableHeight=4 </t>
+  </si>
+  <si>
     <t>check whether the item will fit the truck or not</t>
   </si>
   <si>
+    <t xml:space="preserve">length=4, width=3, height=5, availableLength=8, availableWidth=8, availableHeight=4 </t>
+  </si>
+  <si>
     <t>fail</t>
   </si>
   <si>
     <t>not fit the truck bcz of the height.</t>
   </si>
   <si>
+    <t>length=NULL, width=NULL, height=NULL, availableLength=NULL, availableWidth=NULL, availableHeight= NULL</t>
+  </si>
+  <si>
+    <t>no value assigned.</t>
+  </si>
+  <si>
+    <t>length=10, width=10, height=10, availableLength=5, availableWidth=5, availableHeight=5</t>
+  </si>
+  <si>
     <t>exceeds the max size of truck.</t>
   </si>
   <si>
@@ -435,21 +455,6 @@
     <t>FUNCTION: double distance</t>
   </si>
   <si>
-    <t>T36</t>
-  </si>
-  <si>
-    <t>T37</t>
-  </si>
-  <si>
-    <t>T38</t>
-  </si>
-  <si>
-    <t>T39</t>
-  </si>
-  <si>
-    <t>T40</t>
-  </si>
-  <si>
     <t>Requirement : check user input correct box size</t>
   </si>
   <si>
@@ -555,95 +560,90 @@
     <t>whitebox</t>
   </si>
   <si>
-    <t>space = 15 truck1-&gt;m_totalSpace=8</t>
-  </si>
-  <si>
-    <t>space = 6 truck1-&gt;m_totalSpace=8</t>
-  </si>
-  <si>
-    <t>space = 10 truck1-&gt;m_totalSpace=45</t>
-  </si>
-  <si>
-    <t>space = Null truck1-&gt;m_totalSpace=Null</t>
-  </si>
-  <si>
-    <t>T31</t>
-  </si>
-  <si>
-    <t>T32</t>
-  </si>
-  <si>
-    <t>T33</t>
-  </si>
-  <si>
-    <t>Space = 0</t>
-  </si>
-  <si>
-    <t>Check for negative space = -20</t>
-  </si>
-  <si>
-    <t>Check for maximum space =1</t>
-  </si>
-  <si>
-    <t>no value assigned</t>
-  </si>
-  <si>
-    <t>Truck space remains unchanged, 1 is returned</t>
-  </si>
-  <si>
-    <t>result returned 0</t>
-  </si>
-  <si>
-    <t>1 fail result returned 0</t>
-  </si>
-  <si>
-    <t>T027</t>
-  </si>
-  <si>
-    <t>Whitebox</t>
-  </si>
-  <si>
-    <t>The truck can carry an additional package when it's already near its weight capacity.</t>
-  </si>
-  <si>
-    <t>T028</t>
-  </si>
-  <si>
-    <t>Truck weight = 1000.5 kg, New weight = 199.4 kg</t>
-  </si>
-  <si>
-    <t>Function handles floating-point weights summing close to but not over the weight limit.</t>
-  </si>
-  <si>
-    <t>T029</t>
-  </si>
-  <si>
-    <t>Truck weight = 1000.6 kg, New weight = 199.5 kg</t>
-  </si>
-  <si>
-    <t>T030</t>
-  </si>
-  <si>
-    <t>Truck weight = 1200 kg, New weight = 1 kg</t>
-  </si>
-  <si>
-    <t>Tes+A51+A60:G66</t>
-  </si>
-  <si>
-    <t>Truck weight = 1199 kg, New weight = 1 kg</t>
-  </si>
-  <si>
-    <t>Checks precission with floating-point numbers resulting in total just over the weight limit.</t>
-  </si>
-  <si>
-    <t>A full truck cannot take on even the smallest valid package weight or not</t>
+    <t>Verify that the function correctly identifies the minimum valid box size.</t>
+  </si>
+  <si>
+    <t>Verify that the function correctly identifies the maximum valid box size.</t>
+  </si>
+  <si>
+    <t>Verify that the function correctly handles negative box sizes.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verify that the function correctly identifies a valid box size when the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>shipmentSize</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> parameter matches the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>size3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> constant.</t>
+    </r>
+  </si>
+  <si>
+    <t>T036</t>
+  </si>
+  <si>
+    <t>T037</t>
+  </si>
+  <si>
+    <t>T038</t>
+  </si>
+  <si>
+    <t>T039</t>
+  </si>
+  <si>
+    <t>T040</t>
+  </si>
+  <si>
+    <t>T041</t>
+  </si>
+  <si>
+    <t>T042</t>
+  </si>
+  <si>
+    <t>T043</t>
+  </si>
+  <si>
+    <t>T044</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -656,6 +656,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -768,7 +774,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -795,12 +801,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -825,6 +825,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1159,65 +1166,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5C67FD9-2090-4A05-A979-12107FCFFDB4}">
-  <dimension ref="A1:G75"/>
+  <dimension ref="A1:G78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="112" workbookViewId="0">
+      <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="61.88671875" customWidth="1"/>
-    <col min="4" max="4" width="20.44140625" customWidth="1"/>
-    <col min="5" max="5" width="85.77734375" customWidth="1"/>
-    <col min="6" max="6" width="18.44140625" customWidth="1"/>
-    <col min="7" max="7" width="117.44140625" customWidth="1"/>
+    <col min="3" max="3" width="61.83203125" customWidth="1"/>
+    <col min="4" max="4" width="20.5" customWidth="1"/>
+    <col min="5" max="5" width="85.83203125" customWidth="1"/>
+    <col min="6" max="6" width="18.5" customWidth="1"/>
+    <col min="7" max="7" width="117.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
       <c r="G1" s="11" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="18"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="20" t="s">
+      <c r="D2" s="16"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="20" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="16"/>
-      <c r="B3" s="16"/>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
       <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="4"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="13"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F3" s="19"/>
+      <c r="G3" s="21"/>
+    </row>
+    <row r="4" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
@@ -1237,7 +1244,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>12</v>
       </c>
@@ -1257,7 +1264,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>16</v>
       </c>
@@ -1277,7 +1284,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>21</v>
       </c>
@@ -1297,7 +1304,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>24</v>
       </c>
@@ -1317,12 +1324,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>25</v>
@@ -1337,32 +1344,32 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>29</v>
       </c>
       <c r="B10" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C10" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>147</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>146</v>
       </c>
       <c r="F10" t="s">
         <v>19</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>31</v>
@@ -1374,51 +1381,51 @@
         <v>19</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>31</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="F12" t="s">
         <v>19</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="5"/>
       <c r="G13" s="7"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D14" s="10"/>
       <c r="G14" s="7"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="14" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
       <c r="G15" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -1435,110 +1442,110 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C17" t="s">
         <v>5</v>
       </c>
       <c r="G17" s="7"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B18" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C18" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D18" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E18" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F18" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B19" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C19" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D19" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E19" t="s">
         <v>37</v>
       </c>
       <c r="F19" t="s">
+        <v>155</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>158</v>
+      </c>
+      <c r="B20" t="s">
+        <v>172</v>
+      </c>
+      <c r="C20" t="s">
+        <v>159</v>
+      </c>
+      <c r="D20" t="s">
+        <v>160</v>
+      </c>
+      <c r="E20" t="s">
+        <v>170</v>
+      </c>
+      <c r="F20" t="s">
+        <v>155</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>162</v>
+      </c>
+      <c r="B21" t="s">
+        <v>172</v>
+      </c>
+      <c r="C21" t="s">
+        <v>153</v>
+      </c>
+      <c r="D21" t="s">
+        <v>169</v>
+      </c>
+      <c r="E21" t="s">
         <v>154</v>
       </c>
-      <c r="G19" s="7" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>157</v>
-      </c>
-      <c r="B20" t="s">
-        <v>171</v>
-      </c>
-      <c r="C20" t="s">
-        <v>158</v>
-      </c>
-      <c r="D20" t="s">
-        <v>159</v>
-      </c>
-      <c r="E20" t="s">
-        <v>169</v>
-      </c>
-      <c r="F20" t="s">
-        <v>154</v>
-      </c>
-      <c r="G20" s="7" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>161</v>
-      </c>
-      <c r="B21" t="s">
-        <v>171</v>
-      </c>
-      <c r="C21" t="s">
-        <v>152</v>
-      </c>
-      <c r="D21" t="s">
-        <v>168</v>
-      </c>
-      <c r="E21" t="s">
-        <v>153</v>
-      </c>
       <c r="F21" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>38</v>
       </c>
       <c r="B22" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C22" t="s">
         <v>36</v>
@@ -1553,12 +1560,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>41</v>
       </c>
       <c r="B23" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C23" t="s">
         <v>42</v>
@@ -1573,12 +1580,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>45</v>
       </c>
       <c r="B24" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C24" t="s">
         <v>46</v>
@@ -1593,12 +1600,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>49</v>
       </c>
       <c r="B25" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C25" t="s">
         <v>50</v>
@@ -1613,12 +1620,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>53</v>
       </c>
       <c r="B26" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C26" t="s">
         <v>54</v>
@@ -1633,20 +1640,20 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="B27" s="15"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="B27" s="13"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
       <c r="G27" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>0</v>
       </c>
@@ -1663,7 +1670,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C29" t="s">
         <v>59</v>
       </c>
@@ -1674,9 +1681,9 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="B30" t="s">
         <v>7</v>
@@ -1697,9 +1704,9 @@
         <v>63</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="B31" t="s">
         <v>7</v>
@@ -1720,9 +1727,9 @@
         <v>65</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="B32" t="s">
         <v>7</v>
@@ -1743,9 +1750,9 @@
         <v>67</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="B33" t="s">
         <v>7</v>
@@ -1766,9 +1773,9 @@
         <v>69</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="B34" t="s">
         <v>7</v>
@@ -1789,581 +1796,506 @@
         <v>71</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="B36" s="15"/>
-      <c r="C36" s="15"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="15"/>
-      <c r="F36" s="15"/>
-      <c r="G36" s="1" t="s">
+    <row r="35" spans="1:7" ht="16" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>74</v>
+      </c>
+      <c r="B35" t="s">
+        <v>173</v>
+      </c>
+      <c r="C35" s="22">
+        <v>0.49998999999999999</v>
+      </c>
+      <c r="D35" t="s">
+        <v>62</v>
+      </c>
+      <c r="E35">
+        <v>3</v>
+      </c>
+      <c r="F35" t="s">
+        <v>19</v>
+      </c>
+      <c r="G35" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="16" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>77</v>
+      </c>
+      <c r="B36" t="s">
+        <v>173</v>
+      </c>
+      <c r="C36" s="22">
+        <v>5.0000099999999996</v>
+      </c>
+      <c r="D36" t="s">
+        <v>62</v>
+      </c>
+      <c r="E36">
+        <v>3</v>
+      </c>
+      <c r="F36" t="s">
+        <v>19</v>
+      </c>
+      <c r="G36" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="16" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>79</v>
+      </c>
+      <c r="B37" t="s">
+        <v>173</v>
+      </c>
+      <c r="C37" s="22">
+        <v>-1</v>
+      </c>
+      <c r="D37" t="s">
+        <v>62</v>
+      </c>
+      <c r="E37">
+        <v>3</v>
+      </c>
+      <c r="F37" t="s">
+        <v>19</v>
+      </c>
+      <c r="G37" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="16" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>81</v>
+      </c>
+      <c r="B38" t="s">
+        <v>173</v>
+      </c>
+      <c r="C38" s="22">
+        <v>5</v>
+      </c>
+      <c r="D38" t="s">
+        <v>62</v>
+      </c>
+      <c r="E38">
+        <v>3</v>
+      </c>
+      <c r="F38" t="s">
+        <v>10</v>
+      </c>
+      <c r="G38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="B40" s="13"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="13"/>
+      <c r="G40" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>0</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B41" t="s">
         <v>1</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C41" t="s">
         <v>2</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D41" t="s">
         <v>3</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E41" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+      <c r="F41" t="s">
         <v>73</v>
       </c>
-      <c r="B38" t="s">
-        <v>7</v>
-      </c>
-      <c r="C38" t="s">
-        <v>74</v>
-      </c>
-      <c r="D38" t="s">
-        <v>10</v>
-      </c>
-      <c r="E38" t="s">
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>84</v>
+      </c>
+      <c r="B42" t="s">
+        <v>7</v>
+      </c>
+      <c r="C42" t="s">
         <v>75</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>76</v>
-      </c>
-      <c r="B39" t="s">
-        <v>7</v>
-      </c>
-      <c r="C39" t="s">
-        <v>143</v>
-      </c>
-      <c r="D39" t="s">
-        <v>10</v>
-      </c>
-      <c r="E39" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>78</v>
-      </c>
-      <c r="B40" t="s">
-        <v>7</v>
-      </c>
-      <c r="C40" t="s">
-        <v>144</v>
-      </c>
-      <c r="D40" t="s">
-        <v>19</v>
-      </c>
-      <c r="E40" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>80</v>
-      </c>
-      <c r="B41" t="s">
-        <v>7</v>
-      </c>
-      <c r="C41" t="s">
-        <v>81</v>
-      </c>
-      <c r="D41" t="s">
-        <v>19</v>
-      </c>
-      <c r="E41" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>83</v>
-      </c>
-      <c r="B42" t="s">
-        <v>7</v>
-      </c>
-      <c r="C42" t="s">
-        <v>84</v>
       </c>
       <c r="D42" t="s">
         <v>10</v>
       </c>
       <c r="E42" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>87</v>
+      </c>
+      <c r="B43" t="s">
+        <v>7</v>
+      </c>
+      <c r="C43" t="s">
+        <v>144</v>
+      </c>
+      <c r="D43" t="s">
+        <v>10</v>
+      </c>
+      <c r="E43" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>105</v>
+      </c>
+      <c r="B44" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44" t="s">
+        <v>145</v>
+      </c>
+      <c r="D44" t="s">
+        <v>19</v>
+      </c>
+      <c r="E44" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>106</v>
+      </c>
+      <c r="B45" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45" t="s">
+        <v>82</v>
+      </c>
+      <c r="D45" t="s">
+        <v>19</v>
+      </c>
+      <c r="E45" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>107</v>
+      </c>
+      <c r="B46" t="s">
+        <v>7</v>
+      </c>
+      <c r="C46" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+      <c r="D46" t="s">
+        <v>10</v>
+      </c>
+      <c r="E46" t="s">
         <v>86</v>
       </c>
-      <c r="B43" t="s">
-        <v>7</v>
-      </c>
-      <c r="C43" t="s">
-        <v>87</v>
-      </c>
-      <c r="D43" t="s">
-        <v>19</v>
-      </c>
-      <c r="E43" t="s">
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>108</v>
+      </c>
+      <c r="B47" t="s">
+        <v>7</v>
+      </c>
+      <c r="C47" t="s">
         <v>88</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>187</v>
-      </c>
-      <c r="B44" t="s">
-        <v>188</v>
-      </c>
-      <c r="C44" t="s">
-        <v>198</v>
-      </c>
-      <c r="D44" t="s">
-        <v>10</v>
-      </c>
-      <c r="E44" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>190</v>
-      </c>
-      <c r="B45" t="s">
-        <v>188</v>
-      </c>
-      <c r="C45" t="s">
-        <v>191</v>
-      </c>
-      <c r="D45" t="s">
-        <v>10</v>
-      </c>
-      <c r="E45" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>193</v>
-      </c>
-      <c r="B46" t="s">
-        <v>188</v>
-      </c>
-      <c r="C46" t="s">
-        <v>194</v>
-      </c>
-      <c r="D46" t="s">
-        <v>19</v>
-      </c>
-      <c r="E46" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>195</v>
-      </c>
-      <c r="B47" t="s">
-        <v>188</v>
-      </c>
-      <c r="C47" t="s">
-        <v>196</v>
       </c>
       <c r="D47" t="s">
         <v>19</v>
       </c>
       <c r="E47" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A48" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="B48" s="15"/>
-      <c r="C48" s="15"/>
-      <c r="D48" s="15"/>
-      <c r="E48" s="15"/>
-      <c r="F48" s="15"/>
-      <c r="G48" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A53" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="B53" s="13"/>
+      <c r="C53" s="13"/>
+      <c r="D53" s="13"/>
+      <c r="E53" s="13"/>
+      <c r="F53" s="13"/>
+      <c r="G53" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
         <v>0</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B54" t="s">
         <v>1</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C54" t="s">
         <v>2</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D54" t="s">
         <v>3</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E54" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C50" t="s">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C55" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>109</v>
+      </c>
+      <c r="B56" t="s">
+        <v>7</v>
+      </c>
+      <c r="C56" t="s">
+        <v>91</v>
+      </c>
+      <c r="D56" t="s">
+        <v>10</v>
+      </c>
+      <c r="E56" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>113</v>
+      </c>
+      <c r="B57" t="s">
+        <v>7</v>
+      </c>
+      <c r="C57" t="s">
+        <v>93</v>
+      </c>
+      <c r="D57" t="s">
+        <v>94</v>
+      </c>
+      <c r="E57" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>116</v>
+      </c>
+      <c r="B58" t="s">
+        <v>7</v>
+      </c>
+      <c r="C58" t="s">
+        <v>96</v>
+      </c>
+      <c r="D58" t="s">
+        <v>94</v>
+      </c>
+      <c r="E58" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>119</v>
+      </c>
+      <c r="B59" t="s">
+        <v>7</v>
+      </c>
+      <c r="C59" t="s">
+        <v>98</v>
+      </c>
+      <c r="D59" t="s">
+        <v>94</v>
+      </c>
+      <c r="E59" t="s">
         <v>99</v>
       </c>
-      <c r="B51" t="s">
-        <v>7</v>
-      </c>
-      <c r="C51" t="s">
-        <v>173</v>
-      </c>
-      <c r="D51" t="s">
-        <v>91</v>
-      </c>
-      <c r="E51" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>100</v>
-      </c>
-      <c r="B52" t="s">
-        <v>7</v>
-      </c>
-      <c r="C52" t="s">
-        <v>174</v>
-      </c>
-      <c r="D52" t="s">
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A62" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="B62" s="13"/>
+      <c r="C62" s="13"/>
+      <c r="D62" s="13"/>
+      <c r="E62" s="13"/>
+      <c r="F62" s="13"/>
+      <c r="G62" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>0</v>
+      </c>
+      <c r="B63" t="s">
+        <v>1</v>
+      </c>
+      <c r="C63" t="s">
+        <v>2</v>
+      </c>
+      <c r="F63" t="s">
+        <v>3</v>
+      </c>
+      <c r="G63" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>121</v>
+      </c>
+      <c r="B65" t="s">
+        <v>7</v>
+      </c>
+      <c r="C65" t="s">
+        <v>110</v>
+      </c>
+      <c r="F65" t="s">
+        <v>111</v>
+      </c>
+      <c r="G65" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>178</v>
+      </c>
+      <c r="B66" t="s">
+        <v>7</v>
+      </c>
+      <c r="C66" t="s">
+        <v>114</v>
+      </c>
+      <c r="F66" t="s">
+        <v>111</v>
+      </c>
+      <c r="G66" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>179</v>
+      </c>
+      <c r="B67" t="s">
+        <v>7</v>
+      </c>
+      <c r="C67" t="s">
+        <v>117</v>
+      </c>
+      <c r="F67" t="s">
+        <v>111</v>
+      </c>
+      <c r="G67" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>180</v>
+      </c>
+      <c r="B68" t="s">
+        <v>7</v>
+      </c>
+      <c r="C68" t="s">
+        <v>18</v>
+      </c>
+      <c r="F68" t="s">
+        <v>111</v>
+      </c>
+      <c r="G68" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>181</v>
+      </c>
+      <c r="B69" t="s">
+        <v>7</v>
+      </c>
+      <c r="C69" t="s">
+        <v>122</v>
+      </c>
+      <c r="F69" t="s">
         <v>10</v>
       </c>
-      <c r="E52" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>101</v>
-      </c>
-      <c r="B53" t="s">
-        <v>7</v>
-      </c>
-      <c r="C53" t="s">
-        <v>175</v>
-      </c>
-      <c r="D53" t="s">
-        <v>91</v>
-      </c>
-      <c r="E53" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>102</v>
-      </c>
-      <c r="B54" t="s">
-        <v>7</v>
-      </c>
-      <c r="C54" t="s">
-        <v>176</v>
-      </c>
-      <c r="D54" t="s">
-        <v>91</v>
-      </c>
-      <c r="E54" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>177</v>
-      </c>
-      <c r="B55" t="s">
-        <v>172</v>
-      </c>
-      <c r="C55" t="s">
-        <v>180</v>
-      </c>
-      <c r="D55" t="s">
-        <v>154</v>
-      </c>
-      <c r="E55" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>178</v>
-      </c>
-      <c r="B56" t="s">
-        <v>172</v>
-      </c>
-      <c r="C56" t="s">
-        <v>181</v>
-      </c>
-      <c r="D56" t="s">
-        <v>91</v>
-      </c>
-      <c r="E56" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>179</v>
-      </c>
-      <c r="B57" t="s">
-        <v>172</v>
-      </c>
-      <c r="C57" t="s">
-        <v>182</v>
-      </c>
-      <c r="D57" t="s">
-        <v>91</v>
-      </c>
-      <c r="E57" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A59" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="B59" s="15"/>
-      <c r="C59" s="15"/>
-      <c r="D59" s="15"/>
-      <c r="E59" s="15"/>
-      <c r="F59" s="15"/>
-      <c r="G59" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
-        <v>197</v>
-      </c>
-      <c r="B60" t="s">
+      <c r="G69" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A71" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="B71" s="13"/>
+      <c r="C71" s="13"/>
+      <c r="D71" s="13"/>
+      <c r="E71" s="13"/>
+      <c r="F71" s="13"/>
+      <c r="G71" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>0</v>
+      </c>
+      <c r="B72" t="s">
         <v>1</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C72" t="s">
         <v>2</v>
       </c>
-      <c r="F60" t="s">
-        <v>3</v>
-      </c>
-      <c r="G60" t="s">
+      <c r="D72" t="s">
+        <v>125</v>
+      </c>
+      <c r="E72" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
-        <v>103</v>
-      </c>
-      <c r="B62" t="s">
-        <v>7</v>
-      </c>
-      <c r="C62" t="s">
-        <v>104</v>
-      </c>
-      <c r="F62" t="s">
-        <v>105</v>
-      </c>
-      <c r="G62" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
-        <v>107</v>
-      </c>
-      <c r="B63" t="s">
-        <v>7</v>
-      </c>
-      <c r="C63" t="s">
-        <v>108</v>
-      </c>
-      <c r="F63" t="s">
-        <v>105</v>
-      </c>
-      <c r="G63" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
-        <v>110</v>
-      </c>
-      <c r="B64" t="s">
-        <v>7</v>
-      </c>
-      <c r="C64" t="s">
-        <v>111</v>
-      </c>
-      <c r="F64" t="s">
-        <v>105</v>
-      </c>
-      <c r="G64" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
-        <v>113</v>
-      </c>
-      <c r="B65" t="s">
-        <v>7</v>
-      </c>
-      <c r="C65" t="s">
-        <v>18</v>
-      </c>
-      <c r="F65" t="s">
-        <v>105</v>
-      </c>
-      <c r="G65" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
-        <v>115</v>
-      </c>
-      <c r="B66" t="s">
-        <v>7</v>
-      </c>
-      <c r="C66" t="s">
-        <v>116</v>
-      </c>
-      <c r="F66" t="s">
-        <v>10</v>
-      </c>
-      <c r="G66" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A68" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="B68" s="15"/>
-      <c r="C68" s="15"/>
-      <c r="D68" s="15"/>
-      <c r="E68" s="15"/>
-      <c r="F68" s="15"/>
-      <c r="G68" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
-        <v>0</v>
-      </c>
-      <c r="B69" t="s">
-        <v>1</v>
-      </c>
-      <c r="C69" t="s">
-        <v>2</v>
-      </c>
-      <c r="D69" t="s">
-        <v>119</v>
-      </c>
-      <c r="E69" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C70" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
-        <v>133</v>
-      </c>
-      <c r="B71" t="s">
-        <v>7</v>
-      </c>
-      <c r="C71" t="s">
-        <v>121</v>
-      </c>
-      <c r="D71" t="s">
-        <v>122</v>
-      </c>
-      <c r="E71" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
-        <v>134</v>
-      </c>
-      <c r="B72" t="s">
-        <v>7</v>
-      </c>
-      <c r="C72" t="s">
-        <v>124</v>
-      </c>
-      <c r="D72">
-        <v>6.7</v>
-      </c>
-      <c r="E72" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
-        <v>135</v>
-      </c>
-      <c r="B73" t="s">
-        <v>7</v>
-      </c>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C73" t="s">
         <v>126</v>
       </c>
-      <c r="D73">
-        <v>0</v>
-      </c>
-      <c r="E73" t="s">
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>182</v>
+      </c>
+      <c r="B74" t="s">
+        <v>7</v>
+      </c>
+      <c r="C74" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
-        <v>136</v>
-      </c>
-      <c r="B74" t="s">
-        <v>7</v>
-      </c>
-      <c r="C74" t="s">
+      <c r="D74" t="s">
         <v>128</v>
-      </c>
-      <c r="D74" t="s">
-        <v>122</v>
       </c>
       <c r="E74" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>137</v>
+        <v>183</v>
       </c>
       <c r="B75" t="s">
         <v>7</v>
@@ -2372,26 +2304,77 @@
         <v>130</v>
       </c>
       <c r="D75">
-        <v>35.35</v>
+        <v>6.7</v>
       </c>
       <c r="E75" t="s">
         <v>131</v>
       </c>
     </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>184</v>
+      </c>
+      <c r="B76" t="s">
+        <v>7</v>
+      </c>
+      <c r="C76" t="s">
+        <v>132</v>
+      </c>
+      <c r="D76">
+        <v>0</v>
+      </c>
+      <c r="E76" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>185</v>
+      </c>
+      <c r="B77" t="s">
+        <v>7</v>
+      </c>
+      <c r="C77" t="s">
+        <v>134</v>
+      </c>
+      <c r="D77" t="s">
+        <v>128</v>
+      </c>
+      <c r="E77" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>186</v>
+      </c>
+      <c r="B78" t="s">
+        <v>7</v>
+      </c>
+      <c r="C78" t="s">
+        <v>136</v>
+      </c>
+      <c r="D78">
+        <v>35.35</v>
+      </c>
+      <c r="E78" t="s">
+        <v>137</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="A40:F40"/>
+    <mergeCell ref="A53:F53"/>
+    <mergeCell ref="A62:F62"/>
+    <mergeCell ref="A71:F71"/>
+    <mergeCell ref="A15:F15"/>
+    <mergeCell ref="A27:F27"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="A36:F36"/>
-    <mergeCell ref="A48:F48"/>
-    <mergeCell ref="A59:F59"/>
-    <mergeCell ref="A68:F68"/>
-    <mergeCell ref="A15:F15"/>
-    <mergeCell ref="A27:F27"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update check box size whitebox cases
</commit_message>
<xml_diff>
--- a/Documents/Testing/Tests Documents/Test_case.xlsx
+++ b/Documents/Testing/Tests Documents/Test_case.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jashandeep/Documents/GitHub/winter24--sft221-naa-1/Documents/Testing/Tests Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69328244-2CD2-EA41-8655-514E03C893D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BA9060C-A944-BE4D-99E8-2A3A14835F6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="640" windowWidth="29020" windowHeight="17100" xr2:uid="{16F36B32-E991-4A8C-AA31-131C233A1DED}"/>
   </bookViews>
@@ -801,6 +801,13 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -825,13 +832,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1168,8 +1168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5C67FD9-2090-4A05-A979-12107FCFFDB4}">
   <dimension ref="A1:G78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="112" workbookViewId="0">
-      <selection activeCell="C73" sqref="C73"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="112" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1182,47 +1182,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
       <c r="G1" s="11" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="18" t="s">
+      <c r="D2" s="19"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="13" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
+      <c r="A3" s="17"/>
+      <c r="B3" s="17"/>
       <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="4"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="21"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="14"/>
     </row>
     <row r="4" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
@@ -1413,14 +1413,14 @@
       <c r="G14" s="7"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
       <c r="G15" s="1" t="s">
         <v>35</v>
       </c>
@@ -1641,14 +1641,14 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="12" t="s">
+      <c r="A27" s="15" t="s">
         <v>139</v>
       </c>
-      <c r="B27" s="13"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
       <c r="G27" s="1" t="s">
         <v>58</v>
       </c>
@@ -1803,7 +1803,7 @@
       <c r="B35" t="s">
         <v>173</v>
       </c>
-      <c r="C35" s="22">
+      <c r="C35" s="12">
         <v>0.49998999999999999</v>
       </c>
       <c r="D35" t="s">
@@ -1826,7 +1826,7 @@
       <c r="B36" t="s">
         <v>173</v>
       </c>
-      <c r="C36" s="22">
+      <c r="C36" s="12">
         <v>5.0000099999999996</v>
       </c>
       <c r="D36" t="s">
@@ -1849,7 +1849,7 @@
       <c r="B37" t="s">
         <v>173</v>
       </c>
-      <c r="C37" s="22">
+      <c r="C37" s="12">
         <v>-1</v>
       </c>
       <c r="D37" t="s">
@@ -1872,7 +1872,7 @@
       <c r="B38" t="s">
         <v>173</v>
       </c>
-      <c r="C38" s="22">
+      <c r="C38" s="12">
         <v>5</v>
       </c>
       <c r="D38" t="s">
@@ -1889,14 +1889,14 @@
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" s="12" t="s">
+      <c r="A40" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="B40" s="13"/>
-      <c r="C40" s="13"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="13"/>
-      <c r="F40" s="13"/>
+      <c r="B40" s="16"/>
+      <c r="C40" s="16"/>
+      <c r="D40" s="16"/>
+      <c r="E40" s="16"/>
+      <c r="F40" s="16"/>
       <c r="G40" s="1" t="s">
         <v>72</v>
       </c>
@@ -2024,14 +2024,14 @@
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A53" s="12" t="s">
+      <c r="A53" s="15" t="s">
         <v>141</v>
       </c>
-      <c r="B53" s="13"/>
-      <c r="C53" s="13"/>
-      <c r="D53" s="13"/>
-      <c r="E53" s="13"/>
-      <c r="F53" s="13"/>
+      <c r="B53" s="16"/>
+      <c r="C53" s="16"/>
+      <c r="D53" s="16"/>
+      <c r="E53" s="16"/>
+      <c r="F53" s="16"/>
       <c r="G53" s="1" t="s">
         <v>90</v>
       </c>
@@ -2127,14 +2127,14 @@
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A62" s="12" t="s">
+      <c r="A62" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="B62" s="13"/>
-      <c r="C62" s="13"/>
-      <c r="D62" s="13"/>
-      <c r="E62" s="13"/>
-      <c r="F62" s="13"/>
+      <c r="B62" s="16"/>
+      <c r="C62" s="16"/>
+      <c r="D62" s="16"/>
+      <c r="E62" s="16"/>
+      <c r="F62" s="16"/>
       <c r="G62" s="1" t="s">
         <v>124</v>
       </c>
@@ -2242,14 +2242,14 @@
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A71" s="12" t="s">
+      <c r="A71" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="B71" s="13"/>
-      <c r="C71" s="13"/>
-      <c r="D71" s="13"/>
-      <c r="E71" s="13"/>
-      <c r="F71" s="13"/>
+      <c r="B71" s="16"/>
+      <c r="C71" s="16"/>
+      <c r="D71" s="16"/>
+      <c r="E71" s="16"/>
+      <c r="F71" s="16"/>
       <c r="G71" s="1" t="s">
         <v>138</v>
       </c>
@@ -2363,6 +2363,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:F3"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="A40:F40"/>
     <mergeCell ref="A53:F53"/>
@@ -2370,11 +2375,6 @@
     <mergeCell ref="A71:F71"/>
     <mergeCell ref="A15:F15"/>
     <mergeCell ref="A27:F27"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added checkboxsize whitebox cases
</commit_message>
<xml_diff>
--- a/Documents/Testing/Tests Documents/Test_case.xlsx
+++ b/Documents/Testing/Tests Documents/Test_case.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/84e5bdbfc05febe3/Documents/CPASemester2/SFT221/SFT Project/winter24--sft221-naa-1/Documents/Testing/Tests Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jashandeep/Documents/GitHub/winter24--sft221-naa-1/Documents/Testing/Tests Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="13_ncr:1_{7782F872-E008-4F0E-864F-C667BC6D9785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1FD8A1F4-EA73-4032-BE7E-55D117CB52F9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7CE6E78-C29D-DA4C-9B26-3D2172D9F98E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2184" yWindow="1296" windowWidth="20856" windowHeight="11664" xr2:uid="{16F36B32-E991-4A8C-AA31-131C233A1DED}"/>
+    <workbookView xWindow="2180" yWindow="1300" windowWidth="20860" windowHeight="11660" xr2:uid="{16F36B32-E991-4A8C-AA31-131C233A1DED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="220">
   <si>
     <t>Test #</t>
   </si>
@@ -682,13 +682,65 @@
   </si>
   <si>
     <t xml:space="preserve"> Point p1 = { 'a', '1' };   Point p2 = { 'b', '2' };</t>
+  </si>
+  <si>
+    <t>Verify that the function correctly identifies the minimum valid box size.</t>
+  </si>
+  <si>
+    <t>Verify that the function correctly identifies the maximum valid box size.</t>
+  </si>
+  <si>
+    <t>Verify that the function correctly handles negative box sizes.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verify that the function correctly identifies a valid box size when the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>shipmentSize</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> parameter matches the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>size3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> constant.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -701,6 +753,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -813,7 +871,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -840,12 +898,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -870,6 +922,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1204,65 +1263,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5C67FD9-2090-4A05-A979-12107FCFFDB4}">
-  <dimension ref="A1:G79"/>
+  <dimension ref="A1:G83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B48" workbookViewId="0">
-      <selection activeCell="C81" sqref="C81"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="61.88671875" customWidth="1"/>
-    <col min="4" max="4" width="20.44140625" customWidth="1"/>
-    <col min="5" max="5" width="85.77734375" customWidth="1"/>
-    <col min="6" max="6" width="18.44140625" customWidth="1"/>
-    <col min="7" max="7" width="117.44140625" customWidth="1"/>
+    <col min="3" max="3" width="61.83203125" customWidth="1"/>
+    <col min="4" max="4" width="20.5" customWidth="1"/>
+    <col min="5" max="5" width="85.83203125" customWidth="1"/>
+    <col min="6" max="6" width="18.5" customWidth="1"/>
+    <col min="7" max="7" width="117.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
       <c r="G1" s="11" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="18"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="20" t="s">
+      <c r="D2" s="16"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="20" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="16"/>
-      <c r="B3" s="16"/>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
       <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="4"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="13"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F3" s="19"/>
+      <c r="G3" s="21"/>
+    </row>
+    <row r="4" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
@@ -1282,7 +1341,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>12</v>
       </c>
@@ -1302,7 +1361,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>16</v>
       </c>
@@ -1322,7 +1381,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>21</v>
       </c>
@@ -1342,7 +1401,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>24</v>
       </c>
@@ -1362,7 +1421,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>28</v>
       </c>
@@ -1382,7 +1441,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>29</v>
       </c>
@@ -1402,7 +1461,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>30</v>
       </c>
@@ -1422,7 +1481,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>32</v>
       </c>
@@ -1442,28 +1501,28 @@
         <v>149</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="5"/>
       <c r="G13" s="7"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D14" s="10"/>
       <c r="G14" s="7"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="14" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
       <c r="G15" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -1480,13 +1539,13 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C17" t="s">
         <v>5</v>
       </c>
       <c r="G17" s="7"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>151</v>
       </c>
@@ -1509,7 +1568,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>156</v>
       </c>
@@ -1532,7 +1591,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>157</v>
       </c>
@@ -1555,7 +1614,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>161</v>
       </c>
@@ -1578,7 +1637,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>38</v>
       </c>
@@ -1598,7 +1657,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>41</v>
       </c>
@@ -1618,7 +1677,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>45</v>
       </c>
@@ -1638,7 +1697,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>49</v>
       </c>
@@ -1658,7 +1717,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>53</v>
       </c>
@@ -1678,20 +1737,20 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="14" t="s">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="B27" s="15"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
       <c r="G27" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>0</v>
       </c>
@@ -1708,7 +1767,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C29" t="s">
         <v>59</v>
       </c>
@@ -1719,7 +1778,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>94</v>
       </c>
@@ -1742,7 +1801,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>95</v>
       </c>
@@ -1765,7 +1824,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>96</v>
       </c>
@@ -1788,7 +1847,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>97</v>
       </c>
@@ -1811,7 +1870,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>98</v>
       </c>
@@ -1834,677 +1893,769 @@
         <v>71</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="14" t="s">
+    <row r="35" spans="1:7" ht="16" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>73</v>
+      </c>
+      <c r="B35" t="s">
+        <v>172</v>
+      </c>
+      <c r="C35" s="22">
+        <v>0.49998999999999999</v>
+      </c>
+      <c r="D35" t="s">
+        <v>62</v>
+      </c>
+      <c r="E35">
+        <v>3</v>
+      </c>
+      <c r="F35" t="s">
+        <v>19</v>
+      </c>
+      <c r="G35" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="16" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>76</v>
+      </c>
+      <c r="B36" t="s">
+        <v>172</v>
+      </c>
+      <c r="C36" s="22">
+        <v>5.0000099999999996</v>
+      </c>
+      <c r="D36" t="s">
+        <v>62</v>
+      </c>
+      <c r="E36">
+        <v>3</v>
+      </c>
+      <c r="F36" t="s">
+        <v>19</v>
+      </c>
+      <c r="G36" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="16" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>78</v>
+      </c>
+      <c r="B37" t="s">
+        <v>172</v>
+      </c>
+      <c r="C37" s="22">
+        <v>-1</v>
+      </c>
+      <c r="D37" t="s">
+        <v>62</v>
+      </c>
+      <c r="E37">
+        <v>3</v>
+      </c>
+      <c r="F37" t="s">
+        <v>19</v>
+      </c>
+      <c r="G37" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="16" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>80</v>
+      </c>
+      <c r="B38" t="s">
+        <v>172</v>
+      </c>
+      <c r="C38" s="22">
+        <v>5</v>
+      </c>
+      <c r="D38" t="s">
+        <v>62</v>
+      </c>
+      <c r="E38">
+        <v>3</v>
+      </c>
+      <c r="F38" t="s">
+        <v>10</v>
+      </c>
+      <c r="G38" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" s="12" t="s">
         <v>139</v>
       </c>
-      <c r="B36" s="15"/>
-      <c r="C36" s="15"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="15"/>
-      <c r="F36" s="15"/>
-      <c r="G36" s="1" t="s">
+      <c r="B40" s="13"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="13"/>
+      <c r="G40" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>0</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B41" t="s">
         <v>1</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C41" t="s">
         <v>2</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D41" t="s">
         <v>3</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E41" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>73</v>
       </c>
-      <c r="B38" t="s">
-        <v>7</v>
-      </c>
-      <c r="C38" t="s">
+      <c r="B42" t="s">
+        <v>7</v>
+      </c>
+      <c r="C42" t="s">
         <v>74</v>
-      </c>
-      <c r="D38" t="s">
-        <v>10</v>
-      </c>
-      <c r="E38" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>76</v>
-      </c>
-      <c r="B39" t="s">
-        <v>7</v>
-      </c>
-      <c r="C39" t="s">
-        <v>143</v>
-      </c>
-      <c r="D39" t="s">
-        <v>10</v>
-      </c>
-      <c r="E39" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>78</v>
-      </c>
-      <c r="B40" t="s">
-        <v>7</v>
-      </c>
-      <c r="C40" t="s">
-        <v>144</v>
-      </c>
-      <c r="D40" t="s">
-        <v>19</v>
-      </c>
-      <c r="E40" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>80</v>
-      </c>
-      <c r="B41" t="s">
-        <v>7</v>
-      </c>
-      <c r="C41" t="s">
-        <v>81</v>
-      </c>
-      <c r="D41" t="s">
-        <v>19</v>
-      </c>
-      <c r="E41" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>83</v>
-      </c>
-      <c r="B42" t="s">
-        <v>7</v>
-      </c>
-      <c r="C42" t="s">
-        <v>84</v>
       </c>
       <c r="D42" t="s">
         <v>10</v>
       </c>
       <c r="E42" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>76</v>
+      </c>
+      <c r="B43" t="s">
+        <v>7</v>
+      </c>
+      <c r="C43" t="s">
+        <v>143</v>
+      </c>
+      <c r="D43" t="s">
+        <v>10</v>
+      </c>
+      <c r="E43" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>78</v>
+      </c>
+      <c r="B44" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44" t="s">
+        <v>144</v>
+      </c>
+      <c r="D44" t="s">
+        <v>19</v>
+      </c>
+      <c r="E44" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>80</v>
+      </c>
+      <c r="B45" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45" t="s">
+        <v>81</v>
+      </c>
+      <c r="D45" t="s">
+        <v>19</v>
+      </c>
+      <c r="E45" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>83</v>
+      </c>
+      <c r="B46" t="s">
+        <v>7</v>
+      </c>
+      <c r="C46" t="s">
+        <v>84</v>
+      </c>
+      <c r="D46" t="s">
+        <v>10</v>
+      </c>
+      <c r="E46" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>86</v>
       </c>
-      <c r="B43" t="s">
-        <v>7</v>
-      </c>
-      <c r="C43" t="s">
+      <c r="B47" t="s">
+        <v>7</v>
+      </c>
+      <c r="C47" t="s">
         <v>87</v>
-      </c>
-      <c r="D43" t="s">
-        <v>19</v>
-      </c>
-      <c r="E43" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>187</v>
-      </c>
-      <c r="B44" t="s">
-        <v>188</v>
-      </c>
-      <c r="C44" t="s">
-        <v>198</v>
-      </c>
-      <c r="D44" t="s">
-        <v>10</v>
-      </c>
-      <c r="E44" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>190</v>
-      </c>
-      <c r="B45" t="s">
-        <v>188</v>
-      </c>
-      <c r="C45" t="s">
-        <v>191</v>
-      </c>
-      <c r="D45" t="s">
-        <v>10</v>
-      </c>
-      <c r="E45" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>193</v>
-      </c>
-      <c r="B46" t="s">
-        <v>188</v>
-      </c>
-      <c r="C46" t="s">
-        <v>194</v>
-      </c>
-      <c r="D46" t="s">
-        <v>19</v>
-      </c>
-      <c r="E46" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>195</v>
-      </c>
-      <c r="B47" t="s">
-        <v>188</v>
-      </c>
-      <c r="C47" t="s">
-        <v>196</v>
       </c>
       <c r="D47" t="s">
         <v>19</v>
       </c>
       <c r="E47" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>187</v>
+      </c>
+      <c r="B48" t="s">
+        <v>188</v>
+      </c>
+      <c r="C48" t="s">
+        <v>198</v>
+      </c>
+      <c r="D48" t="s">
+        <v>10</v>
+      </c>
+      <c r="E48" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>190</v>
+      </c>
+      <c r="B49" t="s">
+        <v>188</v>
+      </c>
+      <c r="C49" t="s">
+        <v>191</v>
+      </c>
+      <c r="D49" t="s">
+        <v>10</v>
+      </c>
+      <c r="E49" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>193</v>
+      </c>
+      <c r="B50" t="s">
+        <v>188</v>
+      </c>
+      <c r="C50" t="s">
+        <v>194</v>
+      </c>
+      <c r="D50" t="s">
+        <v>19</v>
+      </c>
+      <c r="E50" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>195</v>
+      </c>
+      <c r="B51" t="s">
+        <v>188</v>
+      </c>
+      <c r="C51" t="s">
+        <v>196</v>
+      </c>
+      <c r="D51" t="s">
+        <v>19</v>
+      </c>
+      <c r="E51" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A48" s="14" t="s">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A52" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="B48" s="15"/>
-      <c r="C48" s="15"/>
-      <c r="D48" s="15"/>
-      <c r="E48" s="15"/>
-      <c r="F48" s="15"/>
-      <c r="G48" s="1" t="s">
+      <c r="B52" s="13"/>
+      <c r="C52" s="13"/>
+      <c r="D52" s="13"/>
+      <c r="E52" s="13"/>
+      <c r="F52" s="13"/>
+      <c r="G52" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
         <v>0</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B53" t="s">
         <v>1</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C53" t="s">
         <v>2</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D53" t="s">
         <v>3</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E53" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C50" t="s">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C54" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
         <v>99</v>
       </c>
-      <c r="B51" t="s">
-        <v>7</v>
-      </c>
-      <c r="C51" t="s">
+      <c r="B55" t="s">
+        <v>7</v>
+      </c>
+      <c r="C55" t="s">
         <v>173</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D55" t="s">
         <v>91</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E55" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
         <v>100</v>
       </c>
-      <c r="B52" t="s">
-        <v>7</v>
-      </c>
-      <c r="C52" t="s">
+      <c r="B56" t="s">
+        <v>7</v>
+      </c>
+      <c r="C56" t="s">
         <v>174</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D56" t="s">
         <v>10</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E56" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
         <v>101</v>
       </c>
-      <c r="B53" t="s">
-        <v>7</v>
-      </c>
-      <c r="C53" t="s">
+      <c r="B57" t="s">
+        <v>7</v>
+      </c>
+      <c r="C57" t="s">
         <v>175</v>
-      </c>
-      <c r="D53" t="s">
-        <v>91</v>
-      </c>
-      <c r="E53" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>102</v>
-      </c>
-      <c r="B54" t="s">
-        <v>7</v>
-      </c>
-      <c r="C54" t="s">
-        <v>176</v>
-      </c>
-      <c r="D54" t="s">
-        <v>91</v>
-      </c>
-      <c r="E54" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>177</v>
-      </c>
-      <c r="B55" t="s">
-        <v>172</v>
-      </c>
-      <c r="C55" t="s">
-        <v>180</v>
-      </c>
-      <c r="D55" t="s">
-        <v>154</v>
-      </c>
-      <c r="E55" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>178</v>
-      </c>
-      <c r="B56" t="s">
-        <v>172</v>
-      </c>
-      <c r="C56" t="s">
-        <v>181</v>
-      </c>
-      <c r="D56" t="s">
-        <v>91</v>
-      </c>
-      <c r="E56" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>179</v>
-      </c>
-      <c r="B57" t="s">
-        <v>172</v>
-      </c>
-      <c r="C57" t="s">
-        <v>182</v>
       </c>
       <c r="D57" t="s">
         <v>91</v>
       </c>
       <c r="E57" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>102</v>
+      </c>
+      <c r="B58" t="s">
+        <v>7</v>
+      </c>
+      <c r="C58" t="s">
+        <v>176</v>
+      </c>
+      <c r="D58" t="s">
+        <v>91</v>
+      </c>
+      <c r="E58" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>177</v>
+      </c>
+      <c r="B59" t="s">
+        <v>172</v>
+      </c>
+      <c r="C59" t="s">
+        <v>180</v>
+      </c>
+      <c r="D59" t="s">
+        <v>154</v>
+      </c>
+      <c r="E59" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>178</v>
+      </c>
+      <c r="B60" t="s">
+        <v>172</v>
+      </c>
+      <c r="C60" t="s">
+        <v>181</v>
+      </c>
+      <c r="D60" t="s">
+        <v>91</v>
+      </c>
+      <c r="E60" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>179</v>
+      </c>
+      <c r="B61" t="s">
+        <v>172</v>
+      </c>
+      <c r="C61" t="s">
+        <v>182</v>
+      </c>
+      <c r="D61" t="s">
+        <v>91</v>
+      </c>
+      <c r="E61" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A59" s="14" t="s">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A63" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="B59" s="15"/>
-      <c r="C59" s="15"/>
-      <c r="D59" s="15"/>
-      <c r="E59" s="15"/>
-      <c r="F59" s="15"/>
-      <c r="G59" s="1" t="s">
+      <c r="B63" s="13"/>
+      <c r="C63" s="13"/>
+      <c r="D63" s="13"/>
+      <c r="E63" s="13"/>
+      <c r="F63" s="13"/>
+      <c r="G63" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
         <v>197</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B64" t="s">
         <v>1</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C64" t="s">
         <v>2</v>
       </c>
-      <c r="F60" t="s">
+      <c r="F64" t="s">
         <v>3</v>
       </c>
-      <c r="G60" t="s">
+      <c r="G64" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
         <v>103</v>
       </c>
-      <c r="B62" t="s">
-        <v>7</v>
-      </c>
-      <c r="C62" t="s">
+      <c r="B66" t="s">
+        <v>7</v>
+      </c>
+      <c r="C66" t="s">
         <v>104</v>
       </c>
-      <c r="F62" t="s">
+      <c r="F66" t="s">
         <v>105</v>
       </c>
-      <c r="G62" t="s">
+      <c r="G66" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
         <v>107</v>
       </c>
-      <c r="B63" t="s">
-        <v>7</v>
-      </c>
-      <c r="C63" t="s">
+      <c r="B67" t="s">
+        <v>7</v>
+      </c>
+      <c r="C67" t="s">
         <v>108</v>
       </c>
-      <c r="F63" t="s">
+      <c r="F67" t="s">
         <v>105</v>
       </c>
-      <c r="G63" t="s">
+      <c r="G67" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
         <v>110</v>
       </c>
-      <c r="B64" t="s">
-        <v>7</v>
-      </c>
-      <c r="C64" t="s">
+      <c r="B68" t="s">
+        <v>7</v>
+      </c>
+      <c r="C68" t="s">
         <v>111</v>
       </c>
-      <c r="F64" t="s">
+      <c r="F68" t="s">
         <v>105</v>
       </c>
-      <c r="G64" t="s">
+      <c r="G68" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
         <v>113</v>
       </c>
-      <c r="B65" t="s">
-        <v>7</v>
-      </c>
-      <c r="C65" t="s">
+      <c r="B69" t="s">
+        <v>7</v>
+      </c>
+      <c r="C69" t="s">
         <v>18</v>
       </c>
-      <c r="F65" t="s">
+      <c r="F69" t="s">
         <v>105</v>
       </c>
-      <c r="G65" t="s">
+      <c r="G69" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
         <v>115</v>
       </c>
-      <c r="B66" t="s">
-        <v>7</v>
-      </c>
-      <c r="C66" t="s">
+      <c r="B70" t="s">
+        <v>7</v>
+      </c>
+      <c r="C70" t="s">
         <v>116</v>
       </c>
-      <c r="F66" t="s">
+      <c r="F70" t="s">
         <v>10</v>
       </c>
-      <c r="G66" t="s">
+      <c r="G70" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A68" s="14" t="s">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A72" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="B68" s="15"/>
-      <c r="C68" s="15"/>
-      <c r="D68" s="15"/>
-      <c r="E68" s="15"/>
-      <c r="F68" s="15"/>
-      <c r="G68" s="1" t="s">
+      <c r="B72" s="13"/>
+      <c r="C72" s="13"/>
+      <c r="D72" s="13"/>
+      <c r="E72" s="13"/>
+      <c r="F72" s="13"/>
+      <c r="G72" s="1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
         <v>0</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B73" t="s">
         <v>1</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C73" t="s">
         <v>2</v>
       </c>
-      <c r="D69" t="s">
+      <c r="D73" t="s">
         <v>119</v>
       </c>
-      <c r="E69" t="s">
+      <c r="E73" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C70" t="s">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C74" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
         <v>133</v>
       </c>
-      <c r="B71" t="s">
-        <v>7</v>
-      </c>
-      <c r="C71" t="s">
+      <c r="B75" t="s">
+        <v>7</v>
+      </c>
+      <c r="C75" t="s">
         <v>121</v>
       </c>
-      <c r="D71" t="s">
+      <c r="D75" t="s">
         <v>122</v>
       </c>
-      <c r="E71" t="s">
+      <c r="E75" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
         <v>134</v>
       </c>
-      <c r="B72" t="s">
-        <v>7</v>
-      </c>
-      <c r="C72" t="s">
+      <c r="B76" t="s">
+        <v>7</v>
+      </c>
+      <c r="C76" t="s">
         <v>124</v>
       </c>
-      <c r="D72">
+      <c r="D76">
         <v>6.7</v>
       </c>
-      <c r="E72" t="s">
+      <c r="E76" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
         <v>135</v>
       </c>
-      <c r="B73" t="s">
-        <v>7</v>
-      </c>
-      <c r="C73" t="s">
+      <c r="B77" t="s">
+        <v>7</v>
+      </c>
+      <c r="C77" t="s">
         <v>126</v>
       </c>
-      <c r="D73">
+      <c r="D77">
         <v>0</v>
       </c>
-      <c r="E73" t="s">
+      <c r="E77" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
         <v>136</v>
       </c>
-      <c r="B74" t="s">
-        <v>7</v>
-      </c>
-      <c r="C74" t="s">
+      <c r="B78" t="s">
+        <v>7</v>
+      </c>
+      <c r="C78" t="s">
         <v>128</v>
       </c>
-      <c r="D74" t="s">
+      <c r="D78" t="s">
         <v>122</v>
       </c>
-      <c r="E74" t="s">
+      <c r="E78" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
         <v>137</v>
       </c>
-      <c r="B75" t="s">
-        <v>7</v>
-      </c>
-      <c r="C75" t="s">
+      <c r="B79" t="s">
+        <v>7</v>
+      </c>
+      <c r="C79" t="s">
         <v>130</v>
       </c>
-      <c r="D75">
+      <c r="D79">
         <v>35.35</v>
       </c>
-      <c r="E75" t="s">
+      <c r="E79" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A76" t="s">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
         <v>203</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B80" t="s">
         <v>188</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C80" t="s">
         <v>201</v>
       </c>
-      <c r="D76" t="s">
+      <c r="D80" t="s">
         <v>202</v>
       </c>
-      <c r="E76" t="s">
+      <c r="E80" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A77" t="s">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
         <v>204</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B81" t="s">
         <v>188</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C81" t="s">
         <v>205</v>
       </c>
-      <c r="D77" t="s">
+      <c r="D81" t="s">
         <v>202</v>
       </c>
-      <c r="E77" t="s">
+      <c r="E81" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A78" t="s">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
         <v>206</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B82" t="s">
         <v>188</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C82" t="s">
         <v>207</v>
       </c>
-      <c r="D78" t="s">
+      <c r="D82" t="s">
         <v>208</v>
       </c>
-      <c r="E78" t="s">
+      <c r="E82" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A79" t="s">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
         <v>212</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B83" t="s">
         <v>188</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C83" t="s">
         <v>215</v>
       </c>
-      <c r="D79" t="s">
+      <c r="D83" t="s">
         <v>214</v>
       </c>
-      <c r="E79" t="s">
+      <c r="E83" t="s">
         <v>213</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="A40:F40"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="A63:F63"/>
+    <mergeCell ref="A72:F72"/>
+    <mergeCell ref="A15:F15"/>
+    <mergeCell ref="A27:F27"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="A36:F36"/>
-    <mergeCell ref="A48:F48"/>
-    <mergeCell ref="A59:F59"/>
-    <mergeCell ref="A68:F68"/>
-    <mergeCell ref="A15:F15"/>
-    <mergeCell ref="A27:F27"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update validdestiantion test case and Whitebox-Unit test
</commit_message>
<xml_diff>
--- a/Documents/Testing/Tests Documents/Test_case.xlsx
+++ b/Documents/Testing/Tests Documents/Test_case.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/84e5bdbfc05febe3/Documents/CPASemester2/SFT221/SFT Project/winter24--sft221-naa-1/Documents/Testing/Tests Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Semeter_2\SFT\Project\MS4\Documents\Testing\Tests Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="87" documentId="13_ncr:1_{7F08CFC2-8F61-ED42-BA19-9636161A1CD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CFCF28D8-24C8-4FBB-A0A3-AB56F5507713}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66079118-6ECB-4E97-AF74-71774F93B432}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{16F36B32-E991-4A8C-AA31-131C233A1DED}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="14580" windowHeight="17370" xr2:uid="{16F36B32-E991-4A8C-AA31-131C233A1DED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="244">
   <si>
     <t>Test #</t>
   </si>
@@ -60,51 +60,24 @@
     <t>Blackbox</t>
   </si>
   <si>
-    <t>Min edge case</t>
-  </si>
-  <si>
-    <t>1A</t>
-  </si>
-  <si>
     <t>Pass</t>
   </si>
   <si>
-    <t>Min valid destination</t>
-  </si>
-  <si>
     <t>T002</t>
   </si>
   <si>
-    <t>Max Edge case</t>
-  </si>
-  <si>
-    <t>24X</t>
-  </si>
-  <si>
-    <t>max valid destination</t>
-  </si>
-  <si>
     <t>T003</t>
   </si>
   <si>
-    <t>Over edge case</t>
-  </si>
-  <si>
     <t>25A</t>
   </si>
   <si>
     <t>Fail</t>
   </si>
   <si>
-    <t>Over edgecase of routemap row</t>
-  </si>
-  <si>
     <t>T004</t>
   </si>
   <si>
-    <t>1Z</t>
-  </si>
-  <si>
     <t>Over edgecase of routemap column</t>
   </si>
   <si>
@@ -114,9 +87,6 @@
     <t>in range</t>
   </si>
   <si>
-    <t>8B</t>
-  </si>
-  <si>
     <t>destination within routemap</t>
   </si>
   <si>
@@ -129,9 +99,6 @@
     <t>T008</t>
   </si>
   <si>
-    <t>invalid</t>
-  </si>
-  <si>
     <t>T009</t>
   </si>
   <si>
@@ -438,16 +405,7 @@
     <t>White box</t>
   </si>
   <si>
-    <t>20Z</t>
-  </si>
-  <si>
     <t>out of column</t>
-  </si>
-  <si>
-    <t>invalid destination because buidling</t>
-  </si>
-  <si>
-    <t>invalid destination because building</t>
   </si>
   <si>
     <t>destination out of map</t>
@@ -791,6 +749,63 @@
   </si>
   <si>
     <t>T015(1)</t>
+  </si>
+  <si>
+    <t>2B</t>
+  </si>
+  <si>
+    <t>Min valid destination in row</t>
+  </si>
+  <si>
+    <t>max valid destination in col</t>
+  </si>
+  <si>
+    <t>8Y</t>
+  </si>
+  <si>
+    <t>Max edgecase of  row</t>
+  </si>
+  <si>
+    <t>Min edge case in row</t>
+  </si>
+  <si>
+    <t>Max Edge case in column</t>
+  </si>
+  <si>
+    <t>Max edge case in row</t>
+  </si>
+  <si>
+    <t>Min edge case in col</t>
+  </si>
+  <si>
+    <t>25B</t>
+  </si>
+  <si>
+    <t>14A</t>
+  </si>
+  <si>
+    <t>in range inside route map is building vaild</t>
+  </si>
+  <si>
+    <t>16M</t>
+  </si>
+  <si>
+    <t>24F</t>
+  </si>
+  <si>
+    <t>30F</t>
+  </si>
+  <si>
+    <t>10H</t>
+  </si>
+  <si>
+    <t>17F</t>
+  </si>
+  <si>
+    <t>invalid inside map but not a building</t>
+  </si>
+  <si>
+    <t>invalid destination because it is not buidling</t>
   </si>
 </sst>
 </file>
@@ -1001,10 +1016,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1326,22 +1337,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5C67FD9-2090-4A05-A979-12107FCFFDB4}">
   <dimension ref="A1:G86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11:G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="3" max="3" width="61.77734375" customWidth="1"/>
-    <col min="4" max="4" width="20.44140625" customWidth="1"/>
-    <col min="5" max="5" width="85.77734375" customWidth="1"/>
-    <col min="6" max="6" width="18.44140625" customWidth="1"/>
-    <col min="7" max="7" width="117.44140625" customWidth="1"/>
+    <col min="3" max="3" width="61.81640625" customWidth="1"/>
+    <col min="4" max="4" width="20.453125" customWidth="1"/>
+    <col min="5" max="5" width="85.81640625" customWidth="1"/>
+    <col min="6" max="6" width="18.453125" customWidth="1"/>
+    <col min="7" max="7" width="117.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="13" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="B1" s="14"/>
       <c r="C1" s="14"/>
@@ -1349,7 +1360,7 @@
       <c r="E1" s="14"/>
       <c r="F1" s="14"/>
       <c r="G1" s="11" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1390,176 +1401,176 @@
         <v>7</v>
       </c>
       <c r="C4" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="F4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" t="s">
-        <v>10</v>
-      </c>
       <c r="G4" s="7" t="s">
-        <v>11</v>
+        <v>226</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>13</v>
+        <v>231</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>14</v>
+        <v>228</v>
       </c>
       <c r="F5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>15</v>
+        <v>227</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="5" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>17</v>
+        <v>232</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>18</v>
+        <v>234</v>
       </c>
       <c r="F6" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>20</v>
+        <v>229</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>17</v>
+        <v>233</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>22</v>
+        <v>235</v>
       </c>
       <c r="F7" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="5" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>26</v>
+        <v>237</v>
       </c>
       <c r="F8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>27</v>
+        <v>236</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="5" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>9</v>
+        <v>238</v>
       </c>
       <c r="F9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="5" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>134</v>
+        <v>239</v>
       </c>
       <c r="F10" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="5" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>31</v>
+        <v>242</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>26</v>
+        <v>240</v>
       </c>
       <c r="F11" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>136</v>
+        <v>243</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="5" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>31</v>
+        <v>242</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>109</v>
+        <v>241</v>
       </c>
       <c r="F12" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>137</v>
+        <v>243</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -1572,7 +1583,7 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="13" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
@@ -1580,7 +1591,7 @@
       <c r="E15" s="14"/>
       <c r="F15" s="14"/>
       <c r="G15" s="1" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1608,199 +1619,199 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>235</v>
+        <v>221</v>
       </c>
       <c r="B18" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
       <c r="C18" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="D18" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="E18" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="F18" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="B19" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
       <c r="C19" t="s">
-        <v>150</v>
+        <v>136</v>
       </c>
       <c r="D19" t="s">
-        <v>151</v>
+        <v>137</v>
       </c>
       <c r="E19" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="F19" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="B20" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
       <c r="C20" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="D20" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="E20" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="F20" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="B21" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
       <c r="C21" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="D21" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
       <c r="E21" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="F21" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="B22" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="C22" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="E22" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="F22" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B23" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="C23" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="E23" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="F23" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>236</v>
+        <v>222</v>
       </c>
       <c r="B24" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="C24" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="E24" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="F24" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
       <c r="B25" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="C25" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="E25" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="F25" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>238</v>
+        <v>224</v>
       </c>
       <c r="B26" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="C26" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="E26" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="F26" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="13" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="B27" s="14"/>
       <c r="C27" s="14"/>
@@ -1808,7 +1819,7 @@
       <c r="E27" s="14"/>
       <c r="F27" s="14"/>
       <c r="G27" s="1" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1830,18 +1841,18 @@
     </row>
     <row r="29" spans="1:7">
       <c r="C29" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="D29" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="E29" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="B30" t="s">
         <v>7</v>
@@ -1850,21 +1861,21 @@
         <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="E30">
         <v>3</v>
       </c>
       <c r="F30" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G30" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="B31" t="s">
         <v>7</v>
@@ -1873,182 +1884,182 @@
         <v>7</v>
       </c>
       <c r="D31" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="E31">
         <v>3</v>
       </c>
       <c r="F31" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G31" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="B32" t="s">
         <v>7</v>
       </c>
       <c r="C32" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="D32" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="E32">
         <v>3</v>
       </c>
       <c r="F32" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G32" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="B33" t="s">
         <v>7</v>
       </c>
       <c r="C33" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="D33" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="E33">
         <v>3</v>
       </c>
       <c r="F33" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G33" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="B34" t="s">
         <v>7</v>
       </c>
       <c r="C34" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="D34" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="E34">
         <v>3</v>
       </c>
       <c r="F34" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G34" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="B35" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="C35" s="12">
         <v>0.49998999999999999</v>
       </c>
       <c r="D35" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="E35">
         <v>3</v>
       </c>
       <c r="F35" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G35" t="s">
-        <v>193</v>
+        <v>179</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="B36" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="C36" s="12">
         <v>5.0000099999999996</v>
       </c>
       <c r="D36" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="E36">
         <v>3</v>
       </c>
       <c r="F36" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G36" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="B37" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="C37" s="12">
         <v>-1</v>
       </c>
       <c r="D37" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="E37">
         <v>3</v>
       </c>
       <c r="F37" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G37" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="B38" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="C38" s="12">
         <v>5</v>
       </c>
       <c r="D38" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="E38">
         <v>3</v>
       </c>
       <c r="F38" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G38" t="s">
-        <v>196</v>
+        <v>182</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="13" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="B40" s="14"/>
       <c r="C40" s="14"/>
@@ -2056,7 +2067,7 @@
       <c r="E40" s="14"/>
       <c r="F40" s="14"/>
       <c r="G40" s="1" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -2078,177 +2089,177 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="B42" t="s">
         <v>7</v>
       </c>
       <c r="C42" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="D42" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E42" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
     </row>
     <row r="43" spans="1:7">
       <c r="A43" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="B43" t="s">
         <v>7</v>
       </c>
       <c r="C43" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="D43" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E43" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
     </row>
     <row r="44" spans="1:7">
       <c r="A44" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="B44" t="s">
         <v>7</v>
       </c>
       <c r="C44" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D44" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E44" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
       <c r="B45" t="s">
         <v>7</v>
       </c>
       <c r="C45" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="D45" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E45" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
     </row>
     <row r="46" spans="1:7">
       <c r="A46" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="B46" t="s">
         <v>7</v>
       </c>
       <c r="C46" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="D46" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E46" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
     </row>
     <row r="47" spans="1:7">
       <c r="A47" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="B47" t="s">
         <v>7</v>
       </c>
       <c r="C47" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="D47" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E47" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="B48" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="C48" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="D48" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E48" t="s">
-        <v>170</v>
+        <v>156</v>
       </c>
     </row>
     <row r="49" spans="1:7">
       <c r="A49" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="B49" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="C49" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="D49" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E49" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
     </row>
     <row r="50" spans="1:7">
       <c r="A50" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
       <c r="B50" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="C50" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="D50" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E50" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
     </row>
     <row r="51" spans="1:7">
       <c r="A51" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="B51" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="C51" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
       <c r="D51" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E51" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
     </row>
     <row r="52" spans="1:7">
       <c r="A52" s="13" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="B52" s="14"/>
       <c r="C52" s="14"/>
@@ -2256,7 +2267,7 @@
       <c r="E52" s="14"/>
       <c r="F52" s="14"/>
       <c r="G52" s="1" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -2278,131 +2289,131 @@
     </row>
     <row r="54" spans="1:7">
       <c r="C54" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="55" spans="1:7">
       <c r="A55" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="B55" t="s">
         <v>7</v>
       </c>
       <c r="C55" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="D55" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="E55" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
     </row>
     <row r="56" spans="1:7">
       <c r="A56" t="s">
-        <v>197</v>
+        <v>183</v>
       </c>
       <c r="B56" t="s">
         <v>7</v>
       </c>
       <c r="C56" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="D56" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E56" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
     </row>
     <row r="57" spans="1:7">
       <c r="A57" t="s">
-        <v>198</v>
+        <v>184</v>
       </c>
       <c r="B57" t="s">
         <v>7</v>
       </c>
       <c r="C57" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="D57" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="E57" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
     </row>
     <row r="58" spans="1:7">
       <c r="A58" t="s">
-        <v>213</v>
+        <v>199</v>
       </c>
       <c r="B58" t="s">
         <v>7</v>
       </c>
       <c r="C58" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="D58" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="E58" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
     </row>
     <row r="59" spans="1:7">
       <c r="A59" t="s">
-        <v>214</v>
+        <v>200</v>
       </c>
       <c r="B59" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="C59" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="D59" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
       <c r="E59" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
     </row>
     <row r="60" spans="1:7">
       <c r="A60" t="s">
-        <v>215</v>
+        <v>201</v>
       </c>
       <c r="B60" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="C60" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="D60" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="E60" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
     </row>
     <row r="61" spans="1:7">
       <c r="A61" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
       <c r="B61" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="C61" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="D61" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="E61" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
     </row>
     <row r="63" spans="1:7">
       <c r="A63" s="13" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="B63" s="14"/>
       <c r="C63" s="14"/>
@@ -2410,12 +2421,12 @@
       <c r="E63" s="14"/>
       <c r="F63" s="14"/>
       <c r="G63" s="1" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
     </row>
     <row r="64" spans="1:7">
       <c r="A64" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="B64" t="s">
         <v>1</v>
@@ -2432,172 +2443,172 @@
     </row>
     <row r="66" spans="1:7">
       <c r="A66" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="B66" t="s">
         <v>7</v>
       </c>
       <c r="C66" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="F66" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="G66" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
     </row>
     <row r="67" spans="1:7">
       <c r="A67" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="B67" t="s">
         <v>7</v>
       </c>
       <c r="C67" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="F67" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="G67" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
     </row>
     <row r="68" spans="1:7">
       <c r="A68" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="B68" t="s">
         <v>7</v>
       </c>
       <c r="C68" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="F68" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="G68" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
     </row>
     <row r="69" spans="1:7">
       <c r="A69" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="B69" t="s">
         <v>7</v>
       </c>
       <c r="C69" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="F69" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="G69" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
     </row>
     <row r="70" spans="1:7">
       <c r="A70" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="B70" t="s">
         <v>7</v>
       </c>
       <c r="C70" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="F70" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G70" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
     </row>
     <row r="71" spans="1:7">
       <c r="A71" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="B71" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="C71" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
       <c r="E71" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
       <c r="F71" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G71" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
     </row>
     <row r="72" spans="1:7">
       <c r="A72" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="B72" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="C72" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="E72" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
       <c r="F72" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="G72" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
     </row>
     <row r="73" spans="1:7">
       <c r="A73" t="s">
-        <v>224</v>
+        <v>210</v>
       </c>
       <c r="B73" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="C73" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
       <c r="E73" t="s">
-        <v>204</v>
+        <v>190</v>
       </c>
       <c r="F73" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G73" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
     </row>
     <row r="74" spans="1:7">
       <c r="A74" t="s">
-        <v>225</v>
+        <v>211</v>
       </c>
       <c r="B74" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="C74" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
       <c r="E74" t="s">
-        <v>210</v>
+        <v>196</v>
       </c>
       <c r="F74" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G74" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
     </row>
     <row r="75" spans="1:7">
       <c r="A75" s="13" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="B75" s="14"/>
       <c r="C75" s="14"/>
@@ -2605,7 +2616,7 @@
       <c r="E75" s="14"/>
       <c r="F75" s="14"/>
       <c r="G75" s="1" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
     </row>
     <row r="76" spans="1:7">
@@ -2619,7 +2630,7 @@
         <v>2</v>
       </c>
       <c r="D76" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="E76" t="s">
         <v>4</v>
@@ -2627,160 +2638,160 @@
     </row>
     <row r="77" spans="1:7">
       <c r="C77" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
     </row>
     <row r="78" spans="1:7">
       <c r="A78" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
       <c r="B78" t="s">
         <v>7</v>
       </c>
       <c r="C78" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="D78" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="E78" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
     </row>
     <row r="79" spans="1:7">
       <c r="A79" t="s">
-        <v>227</v>
+        <v>213</v>
       </c>
       <c r="B79" t="s">
         <v>7</v>
       </c>
       <c r="C79" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="D79">
         <v>6.7</v>
       </c>
       <c r="E79" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
     </row>
     <row r="80" spans="1:7">
       <c r="A80" t="s">
-        <v>228</v>
+        <v>214</v>
       </c>
       <c r="B80" t="s">
         <v>7</v>
       </c>
       <c r="C80" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="D80">
         <v>0</v>
       </c>
       <c r="E80" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="81" spans="1:5">
       <c r="A81" t="s">
-        <v>229</v>
+        <v>215</v>
       </c>
       <c r="B81" t="s">
         <v>7</v>
       </c>
       <c r="C81" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="D81" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="E81" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
     </row>
     <row r="82" spans="1:5">
       <c r="A82" t="s">
-        <v>230</v>
+        <v>216</v>
       </c>
       <c r="B82" t="s">
         <v>7</v>
       </c>
       <c r="C82" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="D82">
         <v>35.35</v>
       </c>
       <c r="E82" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
     </row>
     <row r="83" spans="1:5">
       <c r="A83" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="B83" t="s">
+        <v>155</v>
+      </c>
+      <c r="C83" t="s">
+        <v>168</v>
+      </c>
+      <c r="D83" t="s">
         <v>169</v>
       </c>
-      <c r="C83" t="s">
-        <v>182</v>
-      </c>
-      <c r="D83" t="s">
-        <v>183</v>
-      </c>
       <c r="E83" t="s">
-        <v>187</v>
+        <v>173</v>
       </c>
     </row>
     <row r="84" spans="1:5">
       <c r="A84" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
       <c r="B84" t="s">
+        <v>155</v>
+      </c>
+      <c r="C84" t="s">
+        <v>170</v>
+      </c>
+      <c r="D84" t="s">
         <v>169</v>
       </c>
-      <c r="C84" t="s">
-        <v>184</v>
-      </c>
-      <c r="D84" t="s">
-        <v>183</v>
-      </c>
       <c r="E84" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
     </row>
     <row r="85" spans="1:5">
       <c r="A85" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
       <c r="B85" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="C85" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="D85" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
       <c r="E85" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
     </row>
     <row r="86" spans="1:5">
       <c r="A86" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
       <c r="B86" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="C86" t="s">
-        <v>192</v>
+        <v>178</v>
       </c>
       <c r="D86" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
       <c r="E86" t="s">
-        <v>190</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
integration tests addedd to test cases
</commit_message>
<xml_diff>
--- a/Documents/Testing/Tests Documents/Test_case.xlsx
+++ b/Documents/Testing/Tests Documents/Test_case.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Semeter_2\SFT\Project\MS4\Documents\Testing\Tests Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Antho\OneDrive\Documents\CPASemester2\SFT221\SFT Project\winter24--sft221-naa-1\Documents\Testing\Tests Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFBE8A83-D64E-4EF3-85ED-1D49B09539F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7514E36D-8090-45D9-86C4-2FC357FFF187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="29020" windowHeight="17500" xr2:uid="{16F36B32-E991-4A8C-AA31-131C233A1DED}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{16F36B32-E991-4A8C-AA31-131C233A1DED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="300">
   <si>
     <t>Test #</t>
   </si>
@@ -807,12 +807,210 @@
   <si>
     <t xml:space="preserve"> double distance</t>
   </si>
+  <si>
+    <t>T060</t>
+  </si>
+  <si>
+    <t>Integration Tests</t>
+  </si>
+  <si>
+    <t>T061</t>
+  </si>
+  <si>
+    <t>T062</t>
+  </si>
+  <si>
+    <t>T063</t>
+  </si>
+  <si>
+    <t>T064</t>
+  </si>
+  <si>
+    <t>T065</t>
+  </si>
+  <si>
+    <t>T066</t>
+  </si>
+  <si>
+    <t>T067</t>
+  </si>
+  <si>
+    <t>T068</t>
+  </si>
+  <si>
+    <t>T069</t>
+  </si>
+  <si>
+    <t>T070</t>
+  </si>
+  <si>
+    <t>T071</t>
+  </si>
+  <si>
+    <t>T072</t>
+  </si>
+  <si>
+    <t>T073</t>
+  </si>
+  <si>
+    <t>T074</t>
+  </si>
+  <si>
+    <t>integration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  int weight = 1200;
+  double size = 5.0;
+  char dest[] = "12A";</t>
+  </si>
+  <si>
+    <t>Check to see if the box parameters are correct, pass result to validdestination which will check the destination afterwards. Only check destination if box checks have passed.</t>
+  </si>
+  <si>
+    <t>int weight = 1201;
+double size = 5.0;
+char dest[] = "12A";</t>
+  </si>
+  <si>
+    <t>The test should return true, since all parameters valid</t>
+  </si>
+  <si>
+    <t>The test should return false, since not all  parameters are valid</t>
+  </si>
+  <si>
+    <t>Check to see if the box parameters are correct, weight exceeds limit. Even though destination is correct, it should not be checked based on the return type of the box functions.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> int weight = 1200;
+ double size = 10;
+ char dest[] = "12A";</t>
+  </si>
+  <si>
+    <t>Check to see if the box parameters are correct, size does not match. Even though destination is correct, it should not be checked based on the return type of the box functions.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> int weight = 1200;
+ double size = 10;
+ char dest[] = "25A";</t>
+  </si>
+  <si>
+    <t>Check to see if the box parameters are correct, pass result to validdestination which will check the destination afterwards. Only check destination if box checks have passed. The destination does not contain a building, therefore, it should not be a valid destination.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> int weight = 500;
+ double size = 0.5;
+ char dest[] = "12O";</t>
+  </si>
+  <si>
+    <t>The test should return true, since  all  parameters are valid</t>
+  </si>
+  <si>
+    <t>Check to see if the box parameters are correct, pass result to validdestination which will check the destination afterwards. Only check destination if box checks have passed. The destination contains a building, therefore, it should  be a valid destination.</t>
+  </si>
+  <si>
+    <t>T075</t>
+  </si>
+  <si>
+    <t>T076</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> struct PackageInf package = {0.0,1.0,NULL};
+ struct Truck truck = {0, 0.0,0.0, '\0' };</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> struct PackageInf package = { 0.0,2.0,NULL };
+ struct Truck truck = { 0, 0.0,0.0, '\0' };</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check to see that the package is of correct size. Afterwards,use output of the function to check compatability with the truck by checking the box space available, set to true. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check to see that the package is of correct size, in this case it is not.  Afterwards,use output of the function to check compatability with the truck by checking the box space available, set to false. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> struct PackageInf package = { 0.0,1.0,NULL };
+ struct Truck truck = { 0, 50,0.0, '\0' };</t>
+  </si>
+  <si>
+    <t>Check to see that the package is of correct size. Afterwards,use output of the function to check compatability with the truck by checking the box space available, set to true.  The truck is full for boxspace, so it should not accept the new package.</t>
+  </si>
+  <si>
+    <t>struct PackageInf package = { 0.0,0.5,NULL };
+struct Truck truck = { 0, 49.5,0.0, '\0' };</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check to see that the package is of correct size. Afterwards,use output of the function to check compatability with the truck by checking the box space available, set to true.  We are checking the edge case of the space of the truck, by using decimal numbers and the smallest available box size. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  struct PackageInf package = { -1.0,0.5,NULL };
+  struct Truck truck = { 0, 49.5,0.0, '\0' };</t>
+  </si>
+  <si>
+    <t>Check to see that the package is of correct weight. Afterwards,use output of the function to check compatability with the truck by checking the weight available, set to false.  The weight in the package is invalid here</t>
+  </si>
+  <si>
+    <t>struct PackageInf package = { 50.0,0.5,NULL };
+struct Truck truck = { 0,0.0,1170, '\0' };</t>
+  </si>
+  <si>
+    <t>Check to see that the package is of correct weight. Afterwards,use output of the function to check compatability with the truck by checking the weight available, set to true.  The truck is full for weight, so it should not accept the new package.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> struct PackageInf package = { 50.0,0.5,NULL };
+ struct Truck truck = { 0, 49.5,1150, '\0' };</t>
+  </si>
+  <si>
+    <t>Check to see that the package is of correct weight. Afterwards,use output of the function to check compatability with the truck by checking the weight available, set to true.  We are checking the edge case of the weight of the truck, it should accept the package at the limit of weight available.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> struct PackageInf package = { 1300.0,0.5,NULL };
+ struct Truck truck = { 0, 49.5,1149, '\0' };</t>
+  </si>
+  <si>
+    <t>Check to see that the package is of correct weight. Afterwards,use output of the function to check compatability with the truck by checking the weight available, set to false.  The package is not a correct weight, so the truck should not be checked.</t>
+  </si>
+  <si>
+    <t>T077</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> char dest[] = "12A\0";
+ struct Point destinationPoint;
+ struct Point closestPoint;
+ struct Route blueRoute = getBlueRoute();</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check to see if the destination is valid. Use the output to perform the closestPoint conversions and calculations. The closest point should be correct in terms of the destination point passed. </t>
+  </si>
+  <si>
+    <t>char dest[] = "12Z\0";
+struct Point destinationPoint;
+struct Point closestPoint;
+struct Route blueRoute = getBlueRoute();</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> char dest[] = "11A\0";
+ struct Point destinationPoint;
+ struct Point closestPoint;
+ struct Route blueRoute = getBlueRoute();</t>
+  </si>
+  <si>
+    <t>Check to see if the destination is valid. Use the output to perform the closestPoint conversions and calculations. The point should be recognized as not valid  because it is not a building and therefore, not executed for the calculations</t>
+  </si>
+  <si>
+    <t>Check to see if the destination is valid. Use the output to perform the closestPoint conversions and calculations. The point should be recognized as not valid since it is out of range and therefore, not executed for the calculations</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> char dest[] = "22G\0";
+ struct Point destinationPoint;
+ struct Point closestPoint;
+ struct Route blueRoute = getBlueRoute();</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -943,7 +1141,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -971,6 +1169,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -995,11 +1199,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1335,65 +1536,66 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5C67FD9-2090-4A05-A979-12107FCFFDB4}">
-  <dimension ref="A1:G86"/>
+  <dimension ref="A1:G106"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G75" sqref="G75"/>
+    <sheetView tabSelected="1" topLeftCell="A101" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E110" sqref="E110"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="61.81640625" customWidth="1"/>
-    <col min="4" max="4" width="20.453125" customWidth="1"/>
-    <col min="5" max="5" width="85.81640625" customWidth="1"/>
-    <col min="6" max="6" width="18.453125" customWidth="1"/>
-    <col min="7" max="7" width="117.453125" customWidth="1"/>
+    <col min="2" max="2" width="10.21875" customWidth="1"/>
+    <col min="3" max="3" width="61.77734375" customWidth="1"/>
+    <col min="4" max="4" width="20.44140625" customWidth="1"/>
+    <col min="5" max="5" width="85.77734375" customWidth="1"/>
+    <col min="6" max="6" width="18.44140625" customWidth="1"/>
+    <col min="7" max="7" width="117.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
       <c r="G1" s="11" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="15" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="17"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="19" t="s">
+      <c r="D2" s="19"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="21" t="s">
+      <c r="G2" s="13" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="15"/>
-      <c r="B3" s="15"/>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="17"/>
+      <c r="B3" s="17"/>
       <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="4"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="22"/>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="F3" s="22"/>
+      <c r="G3" s="14"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
@@ -1413,7 +1615,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
@@ -1433,7 +1635,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
@@ -1453,7 +1655,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
@@ -1473,7 +1675,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>15</v>
       </c>
@@ -1493,7 +1695,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>18</v>
       </c>
@@ -1513,7 +1715,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>19</v>
       </c>
@@ -1533,7 +1735,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>20</v>
       </c>
@@ -1553,7 +1755,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>21</v>
       </c>
@@ -1573,28 +1775,28 @@
         <v>236</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="G13" s="7"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D14" s="10"/>
       <c r="G14" s="7"/>
     </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="13" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
       <c r="G15" s="1" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -1611,13 +1813,13 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
         <v>5</v>
       </c>
       <c r="G17" s="7"/>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>214</v>
       </c>
@@ -1640,7 +1842,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -1663,7 +1865,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -1686,7 +1888,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>32</v>
       </c>
@@ -1709,7 +1911,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>36</v>
       </c>
@@ -1729,7 +1931,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>40</v>
       </c>
@@ -1749,7 +1951,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>215</v>
       </c>
@@ -1769,7 +1971,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>216</v>
       </c>
@@ -1789,7 +1991,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>217</v>
       </c>
@@ -1809,20 +2011,20 @@
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
-      <c r="A27" s="13" t="s">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
       <c r="G27" s="1" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>0</v>
       </c>
@@ -1839,7 +2041,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C29" t="s">
         <v>45</v>
       </c>
@@ -1850,7 +2052,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>78</v>
       </c>
@@ -1873,7 +2075,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>79</v>
       </c>
@@ -1896,7 +2098,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>80</v>
       </c>
@@ -1919,7 +2121,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>81</v>
       </c>
@@ -1942,7 +2144,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>82</v>
       </c>
@@ -1965,7 +2167,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>58</v>
       </c>
@@ -1988,7 +2190,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>61</v>
       </c>
@@ -2011,7 +2213,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>63</v>
       </c>
@@ -2034,7 +2236,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>65</v>
       </c>
@@ -2057,20 +2259,20 @@
         <v>175</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
-      <c r="A40" s="13" t="s">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="B40" s="14"/>
-      <c r="C40" s="14"/>
-      <c r="D40" s="14"/>
-      <c r="E40" s="14"/>
-      <c r="F40" s="14"/>
+      <c r="B40" s="16"/>
+      <c r="C40" s="16"/>
+      <c r="D40" s="16"/>
+      <c r="E40" s="16"/>
+      <c r="F40" s="16"/>
       <c r="G40" s="1" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>0</v>
       </c>
@@ -2087,7 +2289,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>68</v>
       </c>
@@ -2104,7 +2306,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>71</v>
       </c>
@@ -2121,7 +2323,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>147</v>
       </c>
@@ -2138,7 +2340,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>150</v>
       </c>
@@ -2155,7 +2357,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>153</v>
       </c>
@@ -2172,7 +2374,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>155</v>
       </c>
@@ -2189,7 +2391,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>186</v>
       </c>
@@ -2206,7 +2408,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>187</v>
       </c>
@@ -2223,7 +2425,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>188</v>
       </c>
@@ -2240,7 +2442,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>90</v>
       </c>
@@ -2257,20 +2459,20 @@
         <v>160</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
-      <c r="A52" s="13" t="s">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A52" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="B52" s="14"/>
-      <c r="C52" s="14"/>
-      <c r="D52" s="14"/>
-      <c r="E52" s="14"/>
-      <c r="F52" s="14"/>
+      <c r="B52" s="16"/>
+      <c r="C52" s="16"/>
+      <c r="D52" s="16"/>
+      <c r="E52" s="16"/>
+      <c r="F52" s="16"/>
       <c r="G52" s="1" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>0</v>
       </c>
@@ -2287,12 +2489,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C54" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>92</v>
       </c>
@@ -2309,7 +2511,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>176</v>
       </c>
@@ -2326,7 +2528,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>177</v>
       </c>
@@ -2343,7 +2545,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>192</v>
       </c>
@@ -2360,7 +2562,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>193</v>
       </c>
@@ -2377,7 +2579,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>194</v>
       </c>
@@ -2394,7 +2596,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>195</v>
       </c>
@@ -2411,20 +2613,20 @@
         <v>146</v>
       </c>
     </row>
-    <row r="63" spans="1:7">
-      <c r="A63" s="13" t="s">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A63" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="B63" s="14"/>
-      <c r="C63" s="14"/>
-      <c r="D63" s="14"/>
-      <c r="E63" s="14"/>
-      <c r="F63" s="14"/>
+      <c r="B63" s="16"/>
+      <c r="C63" s="16"/>
+      <c r="D63" s="16"/>
+      <c r="E63" s="16"/>
+      <c r="F63" s="16"/>
       <c r="G63" s="1" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>157</v>
       </c>
@@ -2441,7 +2643,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:7">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>196</v>
       </c>
@@ -2458,7 +2660,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="67" spans="1:7">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>197</v>
       </c>
@@ -2475,7 +2677,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="68" spans="1:7">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>198</v>
       </c>
@@ -2492,7 +2694,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>199</v>
       </c>
@@ -2509,7 +2711,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="70" spans="1:7">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>200</v>
       </c>
@@ -2526,7 +2728,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="71" spans="1:7">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>201</v>
       </c>
@@ -2546,7 +2748,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="72" spans="1:7">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>202</v>
       </c>
@@ -2566,7 +2768,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="73" spans="1:7">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>203</v>
       </c>
@@ -2586,7 +2788,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="74" spans="1:7">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>204</v>
       </c>
@@ -2606,20 +2808,20 @@
         <v>191</v>
       </c>
     </row>
-    <row r="75" spans="1:7">
-      <c r="A75" s="13" t="s">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A75" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="B75" s="14"/>
-      <c r="C75" s="14"/>
-      <c r="D75" s="14"/>
-      <c r="E75" s="14"/>
-      <c r="F75" s="14"/>
+      <c r="B75" s="16"/>
+      <c r="C75" s="16"/>
+      <c r="D75" s="16"/>
+      <c r="E75" s="16"/>
+      <c r="F75" s="16"/>
       <c r="G75" s="1" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="76" spans="1:7">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>0</v>
       </c>
@@ -2636,12 +2838,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:7">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C77" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="78" spans="1:7">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>205</v>
       </c>
@@ -2658,7 +2860,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="79" spans="1:7">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>206</v>
       </c>
@@ -2675,7 +2877,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="80" spans="1:7">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>207</v>
       </c>
@@ -2692,7 +2894,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="81" spans="1:5">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>208</v>
       </c>
@@ -2709,7 +2911,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="82" spans="1:5">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>209</v>
       </c>
@@ -2726,7 +2928,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="83" spans="1:5">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>210</v>
       </c>
@@ -2743,7 +2945,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="84" spans="1:5">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>211</v>
       </c>
@@ -2760,7 +2962,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="85" spans="1:5">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>212</v>
       </c>
@@ -2777,7 +2979,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="86" spans="1:5">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>213</v>
       </c>
@@ -2794,8 +2996,348 @@
         <v>169</v>
       </c>
     </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A87" s="15" t="s">
+        <v>245</v>
+      </c>
+      <c r="B87" s="16"/>
+      <c r="C87" s="16"/>
+      <c r="D87" s="16"/>
+      <c r="E87" s="16"/>
+      <c r="F87" s="16"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A88" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B88" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C88" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="D88" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="E88" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="F88" s="23"/>
+    </row>
+    <row r="89" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>244</v>
+      </c>
+      <c r="B89" t="s">
+        <v>260</v>
+      </c>
+      <c r="C89" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="D89" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="E89" s="7" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>246</v>
+      </c>
+      <c r="B90" t="s">
+        <v>260</v>
+      </c>
+      <c r="C90" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="D90" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="E90" s="7" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>247</v>
+      </c>
+      <c r="B91" t="s">
+        <v>260</v>
+      </c>
+      <c r="C91" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="D91" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="E91" s="7" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>248</v>
+      </c>
+      <c r="B92" t="s">
+        <v>260</v>
+      </c>
+      <c r="C92" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="D92" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="E92" s="7" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>249</v>
+      </c>
+      <c r="B93" t="s">
+        <v>260</v>
+      </c>
+      <c r="C93" s="7" t="s">
+        <v>271</v>
+      </c>
+      <c r="D93" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="E93" s="7" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>250</v>
+      </c>
+      <c r="B94" t="s">
+        <v>260</v>
+      </c>
+      <c r="C94" s="7" t="s">
+        <v>271</v>
+      </c>
+      <c r="D94" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="E94" s="7" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>251</v>
+      </c>
+      <c r="B95" t="s">
+        <v>260</v>
+      </c>
+      <c r="C95" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="D95" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="E95" s="7" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>252</v>
+      </c>
+      <c r="B96" t="s">
+        <v>260</v>
+      </c>
+      <c r="C96" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="D96" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="E96" s="7" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>253</v>
+      </c>
+      <c r="B97" t="s">
+        <v>260</v>
+      </c>
+      <c r="C97" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="D97" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="E97" s="7" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>254</v>
+      </c>
+      <c r="B98" t="s">
+        <v>260</v>
+      </c>
+      <c r="C98" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="D98" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="E98" s="7" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>255</v>
+      </c>
+      <c r="B99" t="s">
+        <v>260</v>
+      </c>
+      <c r="C99" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="D99" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="E99" s="7" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>256</v>
+      </c>
+      <c r="B100" t="s">
+        <v>260</v>
+      </c>
+      <c r="C100" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="D100" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="E100" s="7" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>257</v>
+      </c>
+      <c r="B101" t="s">
+        <v>260</v>
+      </c>
+      <c r="C101" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="D101" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="E101" s="7" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>258</v>
+      </c>
+      <c r="B102" t="s">
+        <v>260</v>
+      </c>
+      <c r="C102" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="D102" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="E102" s="7" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>259</v>
+      </c>
+      <c r="B103" t="s">
+        <v>260</v>
+      </c>
+      <c r="C103" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="D103" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="E103" s="7" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>274</v>
+      </c>
+      <c r="B104" t="s">
+        <v>260</v>
+      </c>
+      <c r="C104" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="D104" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="E104" s="7" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>275</v>
+      </c>
+      <c r="B105" t="s">
+        <v>260</v>
+      </c>
+      <c r="C105" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="D105" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="E105" s="7" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>292</v>
+      </c>
+      <c r="B106" t="s">
+        <v>260</v>
+      </c>
+      <c r="C106" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="D106" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="E106" s="7" t="s">
+        <v>294</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="13">
+    <mergeCell ref="A87:F87"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:F3"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="A40:F40"/>
     <mergeCell ref="A52:F52"/>
@@ -2803,11 +3345,6 @@
     <mergeCell ref="A75:F75"/>
     <mergeCell ref="A15:F15"/>
     <mergeCell ref="A27:F27"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update traceability matrix with integ tests
</commit_message>
<xml_diff>
--- a/Documents/Testing/Tests Documents/Test_case.xlsx
+++ b/Documents/Testing/Tests Documents/Test_case.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Antho\OneDrive\Documents\CPASemester2\SFT221\SFT Project\winter24--sft221-naa-1\Documents\Testing\Tests Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/84e5bdbfc05febe3/Documents/CPASemester2/SFT221/SFT Project/winter24--sft221-naa-1/Documents/Testing/Tests Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7514E36D-8090-45D9-86C4-2FC357FFF187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="6_{31B67346-CEC5-4014-B7EB-FD72FCC732E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4530C5F0-26A8-4D6E-87B4-2AC5654DC6FF}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{16F36B32-E991-4A8C-AA31-131C233A1DED}"/>
   </bookViews>
@@ -1010,7 +1010,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1169,11 +1169,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1199,8 +1196,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1538,11 +1538,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5C67FD9-2090-4A05-A979-12107FCFFDB4}">
   <dimension ref="A1:G106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E110" sqref="E110"/>
+    <sheetView tabSelected="1" topLeftCell="A89" zoomScale="74" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G95" sqref="G95"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
     <col min="2" max="2" width="10.21875" customWidth="1"/>
     <col min="3" max="3" width="61.77734375" customWidth="1"/>
@@ -1552,50 +1552,50 @@
     <col min="7" max="7" width="117.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:7">
+      <c r="A1" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
       <c r="G1" s="11" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+    <row r="2" spans="1:7">
+      <c r="A2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="21" t="s">
+      <c r="D2" s="18"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="22" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="17"/>
-      <c r="B3" s="17"/>
+    <row r="3" spans="1:7">
+      <c r="A3" s="16"/>
+      <c r="B3" s="16"/>
       <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="4"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="14"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F3" s="21"/>
+      <c r="G3" s="23"/>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
@@ -1615,7 +1615,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7">
       <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
@@ -1635,7 +1635,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7">
       <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
@@ -1655,7 +1655,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7">
       <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
@@ -1675,7 +1675,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7">
       <c r="A8" s="5" t="s">
         <v>15</v>
       </c>
@@ -1695,7 +1695,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7">
       <c r="A9" s="5" t="s">
         <v>18</v>
       </c>
@@ -1715,7 +1715,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7">
       <c r="A10" s="5" t="s">
         <v>19</v>
       </c>
@@ -1735,7 +1735,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7">
       <c r="A11" s="5" t="s">
         <v>20</v>
       </c>
@@ -1755,7 +1755,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7">
       <c r="A12" s="5" t="s">
         <v>21</v>
       </c>
@@ -1775,28 +1775,28 @@
         <v>236</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7">
       <c r="A13" s="5"/>
       <c r="G13" s="7"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7">
       <c r="D14" s="10"/>
       <c r="G14" s="7"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="15" t="s">
+    <row r="15" spans="1:7">
+      <c r="A15" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
       <c r="G15" s="1" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -1813,13 +1813,13 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7">
       <c r="C17" t="s">
         <v>5</v>
       </c>
       <c r="G17" s="7"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>214</v>
       </c>
@@ -1842,7 +1842,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -1865,7 +1865,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -1888,7 +1888,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>32</v>
       </c>
@@ -1911,7 +1911,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>36</v>
       </c>
@@ -1931,7 +1931,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
         <v>40</v>
       </c>
@@ -1951,7 +1951,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7">
       <c r="A24" t="s">
         <v>215</v>
       </c>
@@ -1971,7 +1971,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7">
       <c r="A25" t="s">
         <v>216</v>
       </c>
@@ -1991,7 +1991,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7">
       <c r="A26" t="s">
         <v>217</v>
       </c>
@@ -2011,20 +2011,20 @@
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="15" t="s">
+    <row r="27" spans="1:7">
+      <c r="A27" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="B27" s="16"/>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
       <c r="G27" s="1" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7">
       <c r="A28" t="s">
         <v>0</v>
       </c>
@@ -2041,7 +2041,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7">
       <c r="C29" t="s">
         <v>45</v>
       </c>
@@ -2052,7 +2052,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7">
       <c r="A30" t="s">
         <v>78</v>
       </c>
@@ -2075,7 +2075,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7">
       <c r="A31" t="s">
         <v>79</v>
       </c>
@@ -2098,7 +2098,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7">
       <c r="A32" t="s">
         <v>80</v>
       </c>
@@ -2121,7 +2121,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7">
       <c r="A33" t="s">
         <v>81</v>
       </c>
@@ -2144,7 +2144,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7">
       <c r="A34" t="s">
         <v>82</v>
       </c>
@@ -2167,7 +2167,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7">
       <c r="A35" t="s">
         <v>58</v>
       </c>
@@ -2190,7 +2190,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7">
       <c r="A36" t="s">
         <v>61</v>
       </c>
@@ -2213,7 +2213,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7">
       <c r="A37" t="s">
         <v>63</v>
       </c>
@@ -2236,7 +2236,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7">
       <c r="A38" t="s">
         <v>65</v>
       </c>
@@ -2259,20 +2259,20 @@
         <v>175</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" s="15" t="s">
+    <row r="40" spans="1:7">
+      <c r="A40" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="B40" s="16"/>
-      <c r="C40" s="16"/>
-      <c r="D40" s="16"/>
-      <c r="E40" s="16"/>
-      <c r="F40" s="16"/>
+      <c r="B40" s="15"/>
+      <c r="C40" s="15"/>
+      <c r="D40" s="15"/>
+      <c r="E40" s="15"/>
+      <c r="F40" s="15"/>
       <c r="G40" s="1" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7">
       <c r="A41" t="s">
         <v>0</v>
       </c>
@@ -2289,7 +2289,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7">
       <c r="A42" t="s">
         <v>68</v>
       </c>
@@ -2306,7 +2306,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7">
       <c r="A43" t="s">
         <v>71</v>
       </c>
@@ -2323,7 +2323,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7">
       <c r="A44" t="s">
         <v>147</v>
       </c>
@@ -2340,7 +2340,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7">
       <c r="A45" t="s">
         <v>150</v>
       </c>
@@ -2357,7 +2357,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7">
       <c r="A46" t="s">
         <v>153</v>
       </c>
@@ -2374,7 +2374,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7">
       <c r="A47" t="s">
         <v>155</v>
       </c>
@@ -2391,7 +2391,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7">
       <c r="A48" t="s">
         <v>186</v>
       </c>
@@ -2408,7 +2408,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7">
       <c r="A49" t="s">
         <v>187</v>
       </c>
@@ -2425,7 +2425,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7">
       <c r="A50" t="s">
         <v>188</v>
       </c>
@@ -2442,7 +2442,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7">
       <c r="A51" t="s">
         <v>90</v>
       </c>
@@ -2459,20 +2459,20 @@
         <v>160</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A52" s="15" t="s">
+    <row r="52" spans="1:7">
+      <c r="A52" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="B52" s="16"/>
-      <c r="C52" s="16"/>
-      <c r="D52" s="16"/>
-      <c r="E52" s="16"/>
-      <c r="F52" s="16"/>
+      <c r="B52" s="15"/>
+      <c r="C52" s="15"/>
+      <c r="D52" s="15"/>
+      <c r="E52" s="15"/>
+      <c r="F52" s="15"/>
       <c r="G52" s="1" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7">
       <c r="A53" t="s">
         <v>0</v>
       </c>
@@ -2489,12 +2489,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7">
       <c r="C54" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7">
       <c r="A55" t="s">
         <v>92</v>
       </c>
@@ -2511,7 +2511,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7">
       <c r="A56" t="s">
         <v>176</v>
       </c>
@@ -2528,7 +2528,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7">
       <c r="A57" t="s">
         <v>177</v>
       </c>
@@ -2545,7 +2545,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7">
       <c r="A58" t="s">
         <v>192</v>
       </c>
@@ -2562,7 +2562,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7">
       <c r="A59" t="s">
         <v>193</v>
       </c>
@@ -2579,7 +2579,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7">
       <c r="A60" t="s">
         <v>194</v>
       </c>
@@ -2596,7 +2596,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7">
       <c r="A61" t="s">
         <v>195</v>
       </c>
@@ -2613,20 +2613,20 @@
         <v>146</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A63" s="15" t="s">
+    <row r="63" spans="1:7">
+      <c r="A63" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="B63" s="16"/>
-      <c r="C63" s="16"/>
-      <c r="D63" s="16"/>
-      <c r="E63" s="16"/>
-      <c r="F63" s="16"/>
+      <c r="B63" s="15"/>
+      <c r="C63" s="15"/>
+      <c r="D63" s="15"/>
+      <c r="E63" s="15"/>
+      <c r="F63" s="15"/>
       <c r="G63" s="1" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7">
       <c r="A64" t="s">
         <v>157</v>
       </c>
@@ -2643,7 +2643,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7">
       <c r="A66" t="s">
         <v>196</v>
       </c>
@@ -2660,7 +2660,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7">
       <c r="A67" t="s">
         <v>197</v>
       </c>
@@ -2677,7 +2677,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7">
       <c r="A68" t="s">
         <v>198</v>
       </c>
@@ -2694,7 +2694,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7">
       <c r="A69" t="s">
         <v>199</v>
       </c>
@@ -2711,7 +2711,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7">
       <c r="A70" t="s">
         <v>200</v>
       </c>
@@ -2728,7 +2728,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7">
       <c r="A71" t="s">
         <v>201</v>
       </c>
@@ -2748,7 +2748,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7">
       <c r="A72" t="s">
         <v>202</v>
       </c>
@@ -2768,7 +2768,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7">
       <c r="A73" t="s">
         <v>203</v>
       </c>
@@ -2788,7 +2788,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7">
       <c r="A74" t="s">
         <v>204</v>
       </c>
@@ -2808,20 +2808,20 @@
         <v>191</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A75" s="15" t="s">
+    <row r="75" spans="1:7">
+      <c r="A75" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="B75" s="16"/>
-      <c r="C75" s="16"/>
-      <c r="D75" s="16"/>
-      <c r="E75" s="16"/>
-      <c r="F75" s="16"/>
+      <c r="B75" s="15"/>
+      <c r="C75" s="15"/>
+      <c r="D75" s="15"/>
+      <c r="E75" s="15"/>
+      <c r="F75" s="15"/>
       <c r="G75" s="1" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7">
       <c r="A76" t="s">
         <v>0</v>
       </c>
@@ -2838,12 +2838,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7">
       <c r="C77" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7">
       <c r="A78" t="s">
         <v>205</v>
       </c>
@@ -2860,7 +2860,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7">
       <c r="A79" t="s">
         <v>206</v>
       </c>
@@ -2877,7 +2877,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7">
       <c r="A80" t="s">
         <v>207</v>
       </c>
@@ -2894,7 +2894,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6">
       <c r="A81" t="s">
         <v>208</v>
       </c>
@@ -2911,7 +2911,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6">
       <c r="A82" t="s">
         <v>209</v>
       </c>
@@ -2928,7 +2928,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6">
       <c r="A83" t="s">
         <v>210</v>
       </c>
@@ -2945,7 +2945,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6">
       <c r="A84" t="s">
         <v>211</v>
       </c>
@@ -2962,7 +2962,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6">
       <c r="A85" t="s">
         <v>212</v>
       </c>
@@ -2979,7 +2979,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6">
       <c r="A86" t="s">
         <v>213</v>
       </c>
@@ -2996,35 +2996,35 @@
         <v>169</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A87" s="15" t="s">
+    <row r="87" spans="1:6">
+      <c r="A87" s="14" t="s">
         <v>245</v>
       </c>
-      <c r="B87" s="16"/>
-      <c r="C87" s="16"/>
-      <c r="D87" s="16"/>
-      <c r="E87" s="16"/>
-      <c r="F87" s="16"/>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A88" s="23" t="s">
+      <c r="B87" s="15"/>
+      <c r="C87" s="15"/>
+      <c r="D87" s="15"/>
+      <c r="E87" s="15"/>
+      <c r="F87" s="15"/>
+    </row>
+    <row r="88" spans="1:6">
+      <c r="A88" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B88" s="23" t="s">
+      <c r="B88" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C88" s="23" t="s">
+      <c r="C88" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D88" s="23" t="s">
+      <c r="D88" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="E88" s="23" t="s">
+      <c r="E88" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F88" s="23"/>
-    </row>
-    <row r="89" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="F88" s="13"/>
+    </row>
+    <row r="89" spans="1:6" ht="43.2">
       <c r="A89" t="s">
         <v>244</v>
       </c>
@@ -3041,7 +3041,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" ht="43.2">
       <c r="A90" t="s">
         <v>246</v>
       </c>
@@ -3058,7 +3058,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6" ht="43.2">
       <c r="A91" t="s">
         <v>247</v>
       </c>
@@ -3075,7 +3075,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:6" ht="43.2">
       <c r="A92" t="s">
         <v>248</v>
       </c>
@@ -3092,7 +3092,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="93" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:6" ht="43.2">
       <c r="A93" t="s">
         <v>249</v>
       </c>
@@ -3109,7 +3109,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="94" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6" ht="43.2">
       <c r="A94" t="s">
         <v>250</v>
       </c>
@@ -3126,7 +3126,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="95" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:6" ht="43.2">
       <c r="A95" t="s">
         <v>251</v>
       </c>
@@ -3143,7 +3143,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="96" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:6" ht="43.2">
       <c r="A96" t="s">
         <v>252</v>
       </c>
@@ -3160,7 +3160,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="97" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" ht="43.2">
       <c r="A97" t="s">
         <v>253</v>
       </c>
@@ -3177,7 +3177,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="98" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:5" ht="43.2">
       <c r="A98" t="s">
         <v>254</v>
       </c>
@@ -3194,7 +3194,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="99" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5" ht="43.2">
       <c r="A99" t="s">
         <v>255</v>
       </c>
@@ -3211,7 +3211,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="100" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" ht="43.2">
       <c r="A100" t="s">
         <v>256</v>
       </c>
@@ -3228,7 +3228,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="101" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:5" ht="43.2">
       <c r="A101" t="s">
         <v>257</v>
       </c>
@@ -3245,7 +3245,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="102" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:5" ht="43.2">
       <c r="A102" t="s">
         <v>258</v>
       </c>
@@ -3262,7 +3262,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="103" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:5" ht="57.6">
       <c r="A103" t="s">
         <v>259</v>
       </c>
@@ -3279,7 +3279,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="104" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:5" ht="57.6">
       <c r="A104" t="s">
         <v>274</v>
       </c>
@@ -3296,7 +3296,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="105" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:5" ht="57.6">
       <c r="A105" t="s">
         <v>275</v>
       </c>
@@ -3313,7 +3313,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="106" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:5" ht="57.6">
       <c r="A106" t="s">
         <v>292</v>
       </c>
@@ -3332,12 +3332,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A87:F87"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:F3"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="A40:F40"/>
     <mergeCell ref="A52:F52"/>
@@ -3345,6 +3339,12 @@
     <mergeCell ref="A75:F75"/>
     <mergeCell ref="A15:F15"/>
     <mergeCell ref="A27:F27"/>
+    <mergeCell ref="A87:F87"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated test cases for check box size
</commit_message>
<xml_diff>
--- a/Documents/Testing/Tests Documents/Test_case.xlsx
+++ b/Documents/Testing/Tests Documents/Test_case.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/84e5bdbfc05febe3/Documents/CPASemester2/SFT221/SFT Project/winter24--sft221-naa-1/Documents/Testing/Tests Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jashandeep/Documents/GitHub/winter24--sft221-naa-1/Documents/Testing/Tests Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="6_{31B67346-CEC5-4014-B7EB-FD72FCC732E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4530C5F0-26A8-4D6E-87B4-2AC5654DC6FF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FFC964A-E09C-9C4C-B2C7-15721FF3F495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{16F36B32-E991-4A8C-AA31-131C233A1DED}"/>
+    <workbookView xWindow="3880" yWindow="640" windowWidth="23260" windowHeight="12460" xr2:uid="{16F36B32-E991-4A8C-AA31-131C233A1DED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -183,13 +183,7 @@
     <t xml:space="preserve"> { "0.5","1","5"}</t>
   </si>
   <si>
-    <t>This test case verifies the function's ability to correctly identify a valid box size when the input matches one of the acceptable sizes defined by the constants 'size1', 'size2', or 'size3'. It ensures that the function returns "valid" and 1 (true) as expected.</t>
-  </si>
-  <si>
     <t>{ "0.5","1","5"}</t>
-  </si>
-  <si>
-    <t>This test case evaluates the function's behavior when the input box size exceeds the maximum acceptable size defined by the constants. It verifies that the function properly recognizes such cases as "invalid" and returns 0 (false).</t>
   </si>
   <si>
     <t>2,2</t>
@@ -1005,12 +999,18 @@
  struct Point closestPoint;
  struct Route blueRoute = getBlueRoute();</t>
   </si>
+  <si>
+    <t xml:space="preserve">This test case verifies the function's ability to correctly identify a a random even number for box size and checks if the  input matches one of the acceptable sizes defined by the constants 'size1', 'size2', or 'size3'. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">This test case evaluates the function's behavior when the input box size is random odd number. </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1172,6 +1172,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1195,12 +1201,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1538,64 +1538,64 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5C67FD9-2090-4A05-A979-12107FCFFDB4}">
   <dimension ref="A1:G106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" zoomScale="74" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G95" sqref="G95"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="112" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="10.21875" customWidth="1"/>
-    <col min="3" max="3" width="61.77734375" customWidth="1"/>
-    <col min="4" max="4" width="20.44140625" customWidth="1"/>
-    <col min="5" max="5" width="85.77734375" customWidth="1"/>
-    <col min="6" max="6" width="18.44140625" customWidth="1"/>
-    <col min="7" max="7" width="117.44140625" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" customWidth="1"/>
+    <col min="3" max="3" width="61.83203125" customWidth="1"/>
+    <col min="4" max="4" width="20.5" customWidth="1"/>
+    <col min="5" max="5" width="85.83203125" customWidth="1"/>
+    <col min="6" max="6" width="18.5" customWidth="1"/>
+    <col min="7" max="7" width="117.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
       <c r="G1" s="11" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="16" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="18"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="20" t="s">
+      <c r="D2" s="20"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="G2" s="14" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="16"/>
-      <c r="B3" s="16"/>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="18"/>
+      <c r="B3" s="18"/>
       <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="4"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="23"/>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="F3" s="23"/>
+      <c r="G3" s="15"/>
+    </row>
+    <row r="4" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
@@ -1603,19 +1603,19 @@
         <v>7</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F4" t="s">
         <v>8</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
@@ -1623,19 +1623,19 @@
         <v>7</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F5" t="s">
         <v>8</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
@@ -1643,19 +1643,19 @@
         <v>7</v>
       </c>
       <c r="C6" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>225</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>227</v>
       </c>
       <c r="F6" t="s">
         <v>8</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
@@ -1663,10 +1663,10 @@
         <v>7</v>
       </c>
       <c r="C7" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>226</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>228</v>
       </c>
       <c r="F7" t="s">
         <v>8</v>
@@ -1675,7 +1675,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>15</v>
       </c>
@@ -1686,27 +1686,27 @@
         <v>16</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="F8" t="s">
         <v>8</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="F9" t="s">
         <v>8</v>
@@ -1715,88 +1715,88 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="F10" t="s">
         <v>8</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F11" t="s">
         <v>8</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="F12" t="s">
         <v>8</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="5"/>
       <c r="G13" s="7"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D14" s="10"/>
       <c r="G14" s="7"/>
     </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="14" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
       <c r="G15" s="1" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -1813,110 +1813,110 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C17" t="s">
         <v>5</v>
       </c>
       <c r="G17" s="7"/>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B18" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C18" t="s">
+        <v>123</v>
+      </c>
+      <c r="D18" t="s">
+        <v>124</v>
+      </c>
+      <c r="E18" t="s">
         <v>125</v>
       </c>
-      <c r="D18" t="s">
+      <c r="F18" t="s">
+        <v>118</v>
+      </c>
+      <c r="G18" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="E18" t="s">
-        <v>127</v>
-      </c>
-      <c r="F18" t="s">
-        <v>120</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
+    </row>
+    <row r="19" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C19" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D19" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E19" t="s">
         <v>24</v>
       </c>
       <c r="F19" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>28</v>
       </c>
       <c r="B20" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C20" t="s">
+        <v>120</v>
+      </c>
+      <c r="D20" t="s">
+        <v>121</v>
+      </c>
+      <c r="E20" t="s">
+        <v>130</v>
+      </c>
+      <c r="F20" t="s">
+        <v>118</v>
+      </c>
+      <c r="G20" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="D20" t="s">
-        <v>123</v>
-      </c>
-      <c r="E20" t="s">
-        <v>132</v>
-      </c>
-      <c r="F20" t="s">
-        <v>120</v>
-      </c>
-      <c r="G20" s="7" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
+    </row>
+    <row r="21" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>32</v>
       </c>
       <c r="B21" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C21" t="s">
+        <v>116</v>
+      </c>
+      <c r="D21" t="s">
+        <v>129</v>
+      </c>
+      <c r="E21" t="s">
+        <v>117</v>
+      </c>
+      <c r="F21" t="s">
         <v>118</v>
       </c>
-      <c r="D21" t="s">
-        <v>131</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="G21" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="F21" t="s">
-        <v>120</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
+    </row>
+    <row r="22" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>36</v>
       </c>
       <c r="B22" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C22" t="s">
         <v>23</v>
@@ -1931,12 +1931,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>40</v>
       </c>
       <c r="B23" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C23" t="s">
         <v>29</v>
@@ -1951,12 +1951,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B24" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C24" t="s">
         <v>33</v>
@@ -1971,12 +1971,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B25" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C25" t="s">
         <v>37</v>
@@ -1991,12 +1991,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B26" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C26" t="s">
         <v>41</v>
@@ -2011,20 +2011,20 @@
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
-      <c r="A27" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="B27" s="15"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="B27" s="17"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
       <c r="G27" s="1" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>0</v>
       </c>
@@ -2041,7 +2041,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C29" t="s">
         <v>45</v>
       </c>
@@ -2052,15 +2052,15 @@
         <v>47</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B30" t="s">
         <v>7</v>
       </c>
       <c r="C30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D30" t="s">
         <v>48</v>
@@ -2072,12 +2072,12 @@
         <v>8</v>
       </c>
       <c r="G30" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B31" t="s">
         <v>7</v>
@@ -2086,7 +2086,7 @@
         <v>7</v>
       </c>
       <c r="D31" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E31">
         <v>3</v>
@@ -2095,21 +2095,21 @@
         <v>12</v>
       </c>
       <c r="G31" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B32" t="s">
         <v>7</v>
       </c>
       <c r="C32" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D32" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E32">
         <v>3</v>
@@ -2118,21 +2118,21 @@
         <v>12</v>
       </c>
       <c r="G32" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B33" t="s">
         <v>7</v>
       </c>
       <c r="C33" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D33" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E33">
         <v>3</v>
@@ -2141,21 +2141,21 @@
         <v>12</v>
       </c>
       <c r="G33" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B34" t="s">
         <v>7</v>
       </c>
       <c r="C34" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D34" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E34">
         <v>3</v>
@@ -2164,15 +2164,15 @@
         <v>12</v>
       </c>
       <c r="G34" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="16" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B35" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C35" s="12">
         <v>0.49998999999999999</v>
@@ -2187,15 +2187,15 @@
         <v>12</v>
       </c>
       <c r="G35" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="16" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B36" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C36" s="12">
         <v>5.0000099999999996</v>
@@ -2210,15 +2210,15 @@
         <v>12</v>
       </c>
       <c r="G36" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="16" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B37" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C37" s="12">
         <v>-1</v>
@@ -2233,15 +2233,15 @@
         <v>12</v>
       </c>
       <c r="G37" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="16" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B38" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C38" s="12">
         <v>5</v>
@@ -2256,23 +2256,23 @@
         <v>8</v>
       </c>
       <c r="G38" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7">
-      <c r="A40" s="14" t="s">
-        <v>109</v>
-      </c>
-      <c r="B40" s="15"/>
-      <c r="C40" s="15"/>
-      <c r="D40" s="15"/>
-      <c r="E40" s="15"/>
-      <c r="F40" s="15"/>
+        <v>173</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="B40" s="17"/>
+      <c r="C40" s="17"/>
+      <c r="D40" s="17"/>
+      <c r="E40" s="17"/>
+      <c r="F40" s="17"/>
       <c r="G40" s="1" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>0</v>
       </c>
@@ -2289,190 +2289,190 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B42" t="s">
         <v>7</v>
       </c>
       <c r="C42" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D42" t="s">
         <v>8</v>
       </c>
       <c r="E42" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B43" t="s">
         <v>7</v>
       </c>
       <c r="C43" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D43" t="s">
         <v>8</v>
       </c>
       <c r="E43" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B44" t="s">
         <v>7</v>
       </c>
       <c r="C44" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D44" t="s">
         <v>12</v>
       </c>
       <c r="E44" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B45" t="s">
         <v>7</v>
       </c>
       <c r="C45" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D45" t="s">
         <v>12</v>
       </c>
       <c r="E45" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B46" t="s">
         <v>7</v>
       </c>
       <c r="C46" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D46" t="s">
         <v>8</v>
       </c>
       <c r="E46" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B47" t="s">
         <v>7</v>
       </c>
       <c r="C47" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D47" t="s">
         <v>12</v>
       </c>
       <c r="E47" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B48" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C48" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D48" t="s">
         <v>8</v>
       </c>
       <c r="E48" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>185</v>
+      </c>
+      <c r="B49" t="s">
+        <v>146</v>
+      </c>
+      <c r="C49" t="s">
         <v>149</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7">
-      <c r="A49" t="s">
-        <v>187</v>
-      </c>
-      <c r="B49" t="s">
-        <v>148</v>
-      </c>
-      <c r="C49" t="s">
-        <v>151</v>
       </c>
       <c r="D49" t="s">
         <v>8</v>
       </c>
       <c r="E49" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>186</v>
+      </c>
+      <c r="B50" t="s">
+        <v>146</v>
+      </c>
+      <c r="C50" t="s">
         <v>152</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7">
-      <c r="A50" t="s">
-        <v>188</v>
-      </c>
-      <c r="B50" t="s">
-        <v>148</v>
-      </c>
-      <c r="C50" t="s">
-        <v>154</v>
       </c>
       <c r="D50" t="s">
         <v>12</v>
       </c>
       <c r="E50" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B51" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C51" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D51" t="s">
         <v>12</v>
       </c>
       <c r="E51" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7">
-      <c r="A52" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="B52" s="15"/>
-      <c r="C52" s="15"/>
-      <c r="D52" s="15"/>
-      <c r="E52" s="15"/>
-      <c r="F52" s="15"/>
+        <v>158</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A52" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="B52" s="17"/>
+      <c r="C52" s="17"/>
+      <c r="D52" s="17"/>
+      <c r="E52" s="17"/>
+      <c r="F52" s="17"/>
       <c r="G52" s="1" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>0</v>
       </c>
@@ -2489,146 +2489,146 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C54" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B55" t="s">
         <v>7</v>
       </c>
       <c r="C55" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D55" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E55" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B56" t="s">
         <v>7</v>
       </c>
       <c r="C56" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D56" t="s">
         <v>8</v>
       </c>
       <c r="E56" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B57" t="s">
         <v>7</v>
       </c>
       <c r="C57" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D57" t="s">
+        <v>73</v>
+      </c>
+      <c r="E57" t="s">
         <v>75</v>
       </c>
-      <c r="E57" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7">
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B58" t="s">
         <v>7</v>
       </c>
       <c r="C58" t="s">
+        <v>137</v>
+      </c>
+      <c r="D58" t="s">
+        <v>73</v>
+      </c>
+      <c r="E58" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>191</v>
+      </c>
+      <c r="B59" t="s">
+        <v>133</v>
+      </c>
+      <c r="C59" t="s">
+        <v>138</v>
+      </c>
+      <c r="D59" t="s">
+        <v>118</v>
+      </c>
+      <c r="E59" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>192</v>
+      </c>
+      <c r="B60" t="s">
+        <v>133</v>
+      </c>
+      <c r="C60" t="s">
         <v>139</v>
       </c>
-      <c r="D58" t="s">
-        <v>75</v>
-      </c>
-      <c r="E58" t="s">
+      <c r="D60" t="s">
+        <v>73</v>
+      </c>
+      <c r="E60" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="59" spans="1:7">
-      <c r="A59" t="s">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
         <v>193</v>
       </c>
-      <c r="B59" t="s">
-        <v>135</v>
-      </c>
-      <c r="C59" t="s">
+      <c r="B61" t="s">
+        <v>133</v>
+      </c>
+      <c r="C61" t="s">
         <v>140</v>
       </c>
-      <c r="D59" t="s">
-        <v>120</v>
-      </c>
-      <c r="E59" t="s">
+      <c r="D61" t="s">
+        <v>73</v>
+      </c>
+      <c r="E61" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="60" spans="1:7">
-      <c r="A60" t="s">
-        <v>194</v>
-      </c>
-      <c r="B60" t="s">
-        <v>135</v>
-      </c>
-      <c r="C60" t="s">
-        <v>141</v>
-      </c>
-      <c r="D60" t="s">
-        <v>75</v>
-      </c>
-      <c r="E60" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7">
-      <c r="A61" t="s">
-        <v>195</v>
-      </c>
-      <c r="B61" t="s">
-        <v>135</v>
-      </c>
-      <c r="C61" t="s">
-        <v>142</v>
-      </c>
-      <c r="D61" t="s">
-        <v>75</v>
-      </c>
-      <c r="E61" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7">
-      <c r="A63" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="B63" s="15"/>
-      <c r="C63" s="15"/>
-      <c r="D63" s="15"/>
-      <c r="E63" s="15"/>
-      <c r="F63" s="15"/>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A63" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="B63" s="17"/>
+      <c r="C63" s="17"/>
+      <c r="D63" s="17"/>
+      <c r="E63" s="17"/>
+      <c r="F63" s="17"/>
       <c r="G63" s="1" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B64" t="s">
         <v>1</v>
@@ -2643,60 +2643,60 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:7">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B66" t="s">
         <v>7</v>
       </c>
       <c r="C66" t="s">
+        <v>81</v>
+      </c>
+      <c r="F66" t="s">
+        <v>82</v>
+      </c>
+      <c r="G66" t="s">
         <v>83</v>
       </c>
-      <c r="F66" t="s">
-        <v>84</v>
-      </c>
-      <c r="G66" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7">
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B67" t="s">
         <v>7</v>
       </c>
       <c r="C67" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F67" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G67" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B68" t="s">
         <v>7</v>
       </c>
       <c r="C68" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F68" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G68" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B69" t="s">
         <v>7</v>
@@ -2705,123 +2705,123 @@
         <v>11</v>
       </c>
       <c r="F69" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G69" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B70" t="s">
         <v>7</v>
       </c>
       <c r="C70" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F70" t="s">
         <v>8</v>
       </c>
       <c r="G70" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B71" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C71" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E71" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F71" t="s">
         <v>8</v>
       </c>
       <c r="G71" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>200</v>
+      </c>
+      <c r="B72" t="s">
+        <v>146</v>
+      </c>
+      <c r="C72" t="s">
+        <v>183</v>
+      </c>
+      <c r="E72" t="s">
+        <v>177</v>
+      </c>
+      <c r="F72" t="s">
+        <v>82</v>
+      </c>
+      <c r="G72" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>201</v>
+      </c>
+      <c r="B73" t="s">
+        <v>146</v>
+      </c>
+      <c r="C73" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="72" spans="1:7">
-      <c r="A72" t="s">
-        <v>202</v>
-      </c>
-      <c r="B72" t="s">
-        <v>148</v>
-      </c>
-      <c r="C72" t="s">
-        <v>185</v>
-      </c>
-      <c r="E72" t="s">
-        <v>179</v>
-      </c>
-      <c r="F72" t="s">
-        <v>84</v>
-      </c>
-      <c r="G72" t="s">
+      <c r="E73" t="s">
         <v>181</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7">
-      <c r="A73" t="s">
-        <v>203</v>
-      </c>
-      <c r="B73" t="s">
-        <v>148</v>
-      </c>
-      <c r="C73" t="s">
-        <v>182</v>
-      </c>
-      <c r="E73" t="s">
-        <v>183</v>
       </c>
       <c r="F73" t="s">
         <v>8</v>
       </c>
       <c r="G73" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B74" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C74" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E74" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F74" t="s">
         <v>8</v>
       </c>
       <c r="G74" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7">
-      <c r="A75" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="B75" s="15"/>
-      <c r="C75" s="15"/>
-      <c r="D75" s="15"/>
-      <c r="E75" s="15"/>
-      <c r="F75" s="15"/>
+        <v>189</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A75" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="B75" s="17"/>
+      <c r="C75" s="17"/>
+      <c r="D75" s="17"/>
+      <c r="E75" s="17"/>
+      <c r="F75" s="17"/>
       <c r="G75" s="1" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>0</v>
       </c>
@@ -2832,181 +2832,181 @@
         <v>2</v>
       </c>
       <c r="D76" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E76" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:7">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C77" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B78" t="s">
         <v>7</v>
       </c>
       <c r="C78" t="s">
+        <v>95</v>
+      </c>
+      <c r="D78" t="s">
+        <v>96</v>
+      </c>
+      <c r="E78" t="s">
         <v>97</v>
       </c>
-      <c r="D78" t="s">
-        <v>98</v>
-      </c>
-      <c r="E78" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7">
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B79" t="s">
         <v>7</v>
       </c>
       <c r="C79" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D79">
         <v>6.7</v>
       </c>
       <c r="E79" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B80" t="s">
         <v>7</v>
       </c>
       <c r="C80" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D80">
         <v>0</v>
       </c>
       <c r="E80" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B81" t="s">
         <v>7</v>
       </c>
       <c r="C81" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D81" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E81" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B82" t="s">
         <v>7</v>
       </c>
       <c r="C82" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D82">
         <v>35.35</v>
       </c>
       <c r="E82" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
+        <v>208</v>
+      </c>
+      <c r="B83" t="s">
+        <v>146</v>
+      </c>
+      <c r="C83" t="s">
+        <v>159</v>
+      </c>
+      <c r="D83" t="s">
+        <v>160</v>
+      </c>
+      <c r="E83" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>209</v>
+      </c>
+      <c r="B84" t="s">
+        <v>146</v>
+      </c>
+      <c r="C84" t="s">
+        <v>161</v>
+      </c>
+      <c r="D84" t="s">
+        <v>160</v>
+      </c>
+      <c r="E84" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
         <v>210</v>
       </c>
-      <c r="B83" t="s">
-        <v>148</v>
-      </c>
-      <c r="C83" t="s">
-        <v>161</v>
-      </c>
-      <c r="D83" t="s">
+      <c r="B85" t="s">
+        <v>146</v>
+      </c>
+      <c r="C85" t="s">
         <v>162</v>
       </c>
-      <c r="E83" t="s">
+      <c r="D85" t="s">
+        <v>163</v>
+      </c>
+      <c r="E85" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="84" spans="1:6">
-      <c r="A84" t="s">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
         <v>211</v>
       </c>
-      <c r="B84" t="s">
-        <v>148</v>
-      </c>
-      <c r="C84" t="s">
-        <v>163</v>
-      </c>
-      <c r="D84" t="s">
-        <v>162</v>
-      </c>
-      <c r="E84" t="s">
+      <c r="B86" t="s">
+        <v>146</v>
+      </c>
+      <c r="C86" t="s">
+        <v>169</v>
+      </c>
+      <c r="D86" t="s">
+        <v>168</v>
+      </c>
+      <c r="E86" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="85" spans="1:6">
-      <c r="A85" t="s">
-        <v>212</v>
-      </c>
-      <c r="B85" t="s">
-        <v>148</v>
-      </c>
-      <c r="C85" t="s">
-        <v>164</v>
-      </c>
-      <c r="D85" t="s">
-        <v>165</v>
-      </c>
-      <c r="E85" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6">
-      <c r="A86" t="s">
-        <v>213</v>
-      </c>
-      <c r="B86" t="s">
-        <v>148</v>
-      </c>
-      <c r="C86" t="s">
-        <v>171</v>
-      </c>
-      <c r="D86" t="s">
-        <v>170</v>
-      </c>
-      <c r="E86" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6">
-      <c r="A87" s="14" t="s">
-        <v>245</v>
-      </c>
-      <c r="B87" s="15"/>
-      <c r="C87" s="15"/>
-      <c r="D87" s="15"/>
-      <c r="E87" s="15"/>
-      <c r="F87" s="15"/>
-    </row>
-    <row r="88" spans="1:6">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A87" s="16" t="s">
+        <v>243</v>
+      </c>
+      <c r="B87" s="17"/>
+      <c r="C87" s="17"/>
+      <c r="D87" s="17"/>
+      <c r="E87" s="17"/>
+      <c r="F87" s="17"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" s="13" t="s">
         <v>0</v>
       </c>
@@ -3017,321 +3017,327 @@
         <v>2</v>
       </c>
       <c r="D88" s="13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E88" s="13" t="s">
         <v>4</v>
       </c>
       <c r="F88" s="13"/>
     </row>
-    <row r="89" spans="1:6" ht="43.2">
+    <row r="89" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
+        <v>242</v>
+      </c>
+      <c r="B89" t="s">
+        <v>258</v>
+      </c>
+      <c r="C89" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="D89" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="E89" s="7" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
         <v>244</v>
       </c>
-      <c r="B89" t="s">
-        <v>260</v>
-      </c>
-      <c r="C89" s="7" t="s">
+      <c r="B90" t="s">
+        <v>258</v>
+      </c>
+      <c r="C90" s="7" t="s">
         <v>261</v>
       </c>
-      <c r="D89" s="7" t="s">
+      <c r="D90" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="E90" s="7" t="s">
         <v>264</v>
       </c>
-      <c r="E89" s="7" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" ht="43.2">
-      <c r="A90" t="s">
+    </row>
+    <row r="91" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>245</v>
+      </c>
+      <c r="B91" t="s">
+        <v>258</v>
+      </c>
+      <c r="C91" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="D91" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="E91" s="7" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
         <v>246</v>
       </c>
-      <c r="B90" t="s">
-        <v>260</v>
-      </c>
-      <c r="C90" s="7" t="s">
+      <c r="B92" t="s">
+        <v>258</v>
+      </c>
+      <c r="C92" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="D92" s="7" t="s">
         <v>263</v>
       </c>
-      <c r="D90" s="7" t="s">
-        <v>265</v>
-      </c>
-      <c r="E90" s="7" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" ht="43.2">
-      <c r="A91" t="s">
+      <c r="E92" s="7" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
         <v>247</v>
       </c>
-      <c r="B91" t="s">
-        <v>260</v>
-      </c>
-      <c r="C91" s="7" t="s">
-        <v>267</v>
-      </c>
-      <c r="D91" s="7" t="s">
-        <v>265</v>
-      </c>
-      <c r="E91" s="7" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" ht="43.2">
-      <c r="A92" t="s">
+      <c r="B93" t="s">
+        <v>258</v>
+      </c>
+      <c r="C93" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="D93" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="E93" s="7" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
         <v>248</v>
       </c>
-      <c r="B92" t="s">
-        <v>260</v>
-      </c>
-      <c r="C92" s="7" t="s">
+      <c r="B94" t="s">
+        <v>258</v>
+      </c>
+      <c r="C94" s="7" t="s">
         <v>269</v>
       </c>
-      <c r="D92" s="7" t="s">
-        <v>265</v>
-      </c>
-      <c r="E92" s="7" t="s">
+      <c r="D94" s="7" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="93" spans="1:6" ht="43.2">
-      <c r="A93" t="s">
+      <c r="E94" s="7" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
         <v>249</v>
       </c>
-      <c r="B93" t="s">
-        <v>260</v>
-      </c>
-      <c r="C93" s="7" t="s">
-        <v>271</v>
-      </c>
-      <c r="D93" s="7" t="s">
+      <c r="B95" t="s">
+        <v>258</v>
+      </c>
+      <c r="C95" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="D95" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="E95" s="7" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>250</v>
+      </c>
+      <c r="B96" t="s">
+        <v>258</v>
+      </c>
+      <c r="C96" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="D96" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="E96" s="7" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>251</v>
+      </c>
+      <c r="B97" t="s">
+        <v>258</v>
+      </c>
+      <c r="C97" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="D97" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="E97" s="7" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>252</v>
+      </c>
+      <c r="B98" t="s">
+        <v>258</v>
+      </c>
+      <c r="C98" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="D98" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="E98" s="7" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>253</v>
+      </c>
+      <c r="B99" t="s">
+        <v>258</v>
+      </c>
+      <c r="C99" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="D99" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="E99" s="7" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>254</v>
+      </c>
+      <c r="B100" t="s">
+        <v>258</v>
+      </c>
+      <c r="C100" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="D100" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="E100" s="7" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>255</v>
+      </c>
+      <c r="B101" t="s">
+        <v>258</v>
+      </c>
+      <c r="C101" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="D101" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="E101" s="7" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>256</v>
+      </c>
+      <c r="B102" t="s">
+        <v>258</v>
+      </c>
+      <c r="C102" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="D102" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="E102" s="7" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>257</v>
+      </c>
+      <c r="B103" t="s">
+        <v>258</v>
+      </c>
+      <c r="C103" s="7" t="s">
+        <v>291</v>
+      </c>
+      <c r="D103" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="E103" s="7" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
         <v>272</v>
       </c>
-      <c r="E93" s="7" t="s">
+      <c r="B104" t="s">
+        <v>258</v>
+      </c>
+      <c r="C104" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="D104" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="E104" s="7" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="94" spans="1:6" ht="43.2">
-      <c r="A94" t="s">
-        <v>250</v>
-      </c>
-      <c r="B94" t="s">
-        <v>260</v>
-      </c>
-      <c r="C94" s="7" t="s">
-        <v>271</v>
-      </c>
-      <c r="D94" s="7" t="s">
-        <v>272</v>
-      </c>
-      <c r="E94" s="7" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" ht="43.2">
-      <c r="A95" t="s">
-        <v>251</v>
-      </c>
-      <c r="B95" t="s">
-        <v>260</v>
-      </c>
-      <c r="C95" s="7" t="s">
-        <v>276</v>
-      </c>
-      <c r="D95" s="7" t="s">
-        <v>272</v>
-      </c>
-      <c r="E95" s="7" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" ht="43.2">
-      <c r="A96" t="s">
-        <v>252</v>
-      </c>
-      <c r="B96" t="s">
-        <v>260</v>
-      </c>
-      <c r="C96" s="7" t="s">
-        <v>277</v>
-      </c>
-      <c r="D96" s="7" t="s">
-        <v>265</v>
-      </c>
-      <c r="E96" s="7" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" ht="43.2">
-      <c r="A97" t="s">
-        <v>253</v>
-      </c>
-      <c r="B97" t="s">
-        <v>260</v>
-      </c>
-      <c r="C97" s="7" t="s">
-        <v>280</v>
-      </c>
-      <c r="D97" s="7" t="s">
-        <v>265</v>
-      </c>
-      <c r="E97" s="7" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" ht="43.2">
-      <c r="A98" t="s">
-        <v>254</v>
-      </c>
-      <c r="B98" t="s">
-        <v>260</v>
-      </c>
-      <c r="C98" s="7" t="s">
-        <v>282</v>
-      </c>
-      <c r="D98" s="7" t="s">
-        <v>272</v>
-      </c>
-      <c r="E98" s="7" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" ht="43.2">
-      <c r="A99" t="s">
-        <v>255</v>
-      </c>
-      <c r="B99" t="s">
-        <v>260</v>
-      </c>
-      <c r="C99" s="7" t="s">
-        <v>284</v>
-      </c>
-      <c r="D99" s="7" t="s">
-        <v>265</v>
-      </c>
-      <c r="E99" s="7" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" ht="43.2">
-      <c r="A100" t="s">
-        <v>256</v>
-      </c>
-      <c r="B100" t="s">
-        <v>260</v>
-      </c>
-      <c r="C100" s="7" t="s">
-        <v>286</v>
-      </c>
-      <c r="D100" s="7" t="s">
-        <v>265</v>
-      </c>
-      <c r="E100" s="7" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" ht="43.2">
-      <c r="A101" t="s">
-        <v>257</v>
-      </c>
-      <c r="B101" t="s">
-        <v>260</v>
-      </c>
-      <c r="C101" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="D101" s="7" t="s">
-        <v>272</v>
-      </c>
-      <c r="E101" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" ht="43.2">
-      <c r="A102" t="s">
+      <c r="B105" t="s">
         <v>258</v>
       </c>
-      <c r="B102" t="s">
-        <v>260</v>
-      </c>
-      <c r="C102" s="7" t="s">
+      <c r="C105" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="D105" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="E105" s="7" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
         <v>290</v>
       </c>
-      <c r="D102" s="7" t="s">
-        <v>265</v>
-      </c>
-      <c r="E102" s="7" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" ht="57.6">
-      <c r="A103" t="s">
-        <v>259</v>
-      </c>
-      <c r="B103" t="s">
-        <v>260</v>
-      </c>
-      <c r="C103" s="7" t="s">
-        <v>293</v>
-      </c>
-      <c r="D103" s="7" t="s">
-        <v>272</v>
-      </c>
-      <c r="E103" s="7" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" ht="57.6">
-      <c r="A104" t="s">
-        <v>274</v>
-      </c>
-      <c r="B104" t="s">
-        <v>260</v>
-      </c>
-      <c r="C104" s="7" t="s">
-        <v>295</v>
-      </c>
-      <c r="D104" s="7" t="s">
-        <v>265</v>
-      </c>
-      <c r="E104" s="7" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" ht="57.6">
-      <c r="A105" t="s">
-        <v>275</v>
-      </c>
-      <c r="B105" t="s">
-        <v>260</v>
-      </c>
-      <c r="C105" s="7" t="s">
-        <v>296</v>
-      </c>
-      <c r="D105" s="7" t="s">
-        <v>265</v>
-      </c>
-      <c r="E105" s="7" t="s">
+      <c r="B106" t="s">
+        <v>258</v>
+      </c>
+      <c r="C106" s="7" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="106" spans="1:5" ht="57.6">
-      <c r="A106" t="s">
+      <c r="D106" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="E106" s="7" t="s">
         <v>292</v>
-      </c>
-      <c r="B106" t="s">
-        <v>260</v>
-      </c>
-      <c r="C106" s="7" t="s">
-        <v>299</v>
-      </c>
-      <c r="D106" s="7" t="s">
-        <v>272</v>
-      </c>
-      <c r="E106" s="7" t="s">
-        <v>294</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A87:F87"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:F3"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="A40:F40"/>
     <mergeCell ref="A52:F52"/>
@@ -3339,12 +3345,6 @@
     <mergeCell ref="A75:F75"/>
     <mergeCell ref="A15:F15"/>
     <mergeCell ref="A27:F27"/>
-    <mergeCell ref="A87:F87"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Acceptance - color up - updating - traceability matrix
</commit_message>
<xml_diff>
--- a/Documents/Testing/Tests Documents/Test_case.xlsx
+++ b/Documents/Testing/Tests Documents/Test_case.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jashandeep/Documents/GitHub/winter24--sft221-naa-1/Documents/Testing/Tests Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Semeter_2\SFT\MS4\Documents\Testing\Tests Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37076827-4500-8747-829A-3BE506F54781}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31BF6A6C-84B8-4BA2-B690-BC4E98B3B3A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3880" yWindow="640" windowWidth="23260" windowHeight="12460" xr2:uid="{16F36B32-E991-4A8C-AA31-131C233A1DED}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="29020" windowHeight="17500" xr2:uid="{16F36B32-E991-4A8C-AA31-131C233A1DED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1010,7 +1010,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1172,12 +1172,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1201,6 +1195,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1538,64 +1538,64 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5C67FD9-2090-4A05-A979-12107FCFFDB4}">
   <dimension ref="A1:G106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F25" zoomScale="112" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="112" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="10.1640625" customWidth="1"/>
-    <col min="3" max="3" width="61.83203125" customWidth="1"/>
-    <col min="4" max="4" width="20.5" customWidth="1"/>
-    <col min="5" max="5" width="85.83203125" customWidth="1"/>
-    <col min="6" max="6" width="18.5" customWidth="1"/>
-    <col min="7" max="7" width="117.5" customWidth="1"/>
+    <col min="2" max="2" width="10.1796875" customWidth="1"/>
+    <col min="3" max="3" width="61.81640625" customWidth="1"/>
+    <col min="4" max="4" width="20.453125" customWidth="1"/>
+    <col min="5" max="5" width="85.81640625" customWidth="1"/>
+    <col min="6" max="6" width="18.453125" customWidth="1"/>
+    <col min="7" max="7" width="117.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:7">
+      <c r="A1" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
       <c r="G1" s="11" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="18" t="s">
+    <row r="2" spans="1:7">
+      <c r="A2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="20"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="22" t="s">
+      <c r="D2" s="18"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="22" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="18"/>
-      <c r="B3" s="18"/>
+    <row r="3" spans="1:7">
+      <c r="A3" s="16"/>
+      <c r="B3" s="16"/>
       <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="4"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="15"/>
-    </row>
-    <row r="4" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="F3" s="21"/>
+      <c r="G3" s="23"/>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
@@ -1615,7 +1615,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7">
       <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
@@ -1635,7 +1635,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7">
       <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
@@ -1655,7 +1655,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7">
       <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
@@ -1675,7 +1675,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7">
       <c r="A8" s="5" t="s">
         <v>15</v>
       </c>
@@ -1695,7 +1695,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7">
       <c r="A9" s="5" t="s">
         <v>18</v>
       </c>
@@ -1715,7 +1715,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7">
       <c r="A10" s="5" t="s">
         <v>19</v>
       </c>
@@ -1735,7 +1735,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7">
       <c r="A11" s="5" t="s">
         <v>20</v>
       </c>
@@ -1755,7 +1755,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7">
       <c r="A12" s="5" t="s">
         <v>21</v>
       </c>
@@ -1775,28 +1775,28 @@
         <v>232</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7">
       <c r="A13" s="5"/>
       <c r="G13" s="7"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7">
       <c r="D14" s="10"/>
       <c r="G14" s="7"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="16" t="s">
+    <row r="15" spans="1:7">
+      <c r="A15" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
       <c r="G15" s="1" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -1813,13 +1813,13 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7">
       <c r="C17" t="s">
         <v>5</v>
       </c>
       <c r="G17" s="7"/>
     </row>
-    <row r="18" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>210</v>
       </c>
@@ -1842,7 +1842,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -1865,7 +1865,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -1888,7 +1888,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>32</v>
       </c>
@@ -1911,7 +1911,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>36</v>
       </c>
@@ -1931,7 +1931,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
         <v>40</v>
       </c>
@@ -1951,7 +1951,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7">
       <c r="A24" t="s">
         <v>211</v>
       </c>
@@ -1971,7 +1971,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7">
       <c r="A25" t="s">
         <v>212</v>
       </c>
@@ -1991,7 +1991,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7">
       <c r="A26" t="s">
         <v>213</v>
       </c>
@@ -2011,20 +2011,20 @@
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="16" t="s">
+    <row r="27" spans="1:7">
+      <c r="A27" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="B27" s="17"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="17"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
       <c r="G27" s="1" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7">
       <c r="A28" t="s">
         <v>0</v>
       </c>
@@ -2041,7 +2041,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7">
       <c r="C29" t="s">
         <v>45</v>
       </c>
@@ -2052,7 +2052,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7">
       <c r="A30" t="s">
         <v>76</v>
       </c>
@@ -2075,7 +2075,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7">
       <c r="A31" t="s">
         <v>77</v>
       </c>
@@ -2098,7 +2098,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7">
       <c r="A32" t="s">
         <v>78</v>
       </c>
@@ -2121,7 +2121,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7">
       <c r="A33" t="s">
         <v>79</v>
       </c>
@@ -2144,7 +2144,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7">
       <c r="A34" t="s">
         <v>80</v>
       </c>
@@ -2167,7 +2167,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7">
       <c r="A35" t="s">
         <v>56</v>
       </c>
@@ -2190,7 +2190,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7">
       <c r="A36" t="s">
         <v>59</v>
       </c>
@@ -2213,7 +2213,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7">
       <c r="A37" t="s">
         <v>61</v>
       </c>
@@ -2236,7 +2236,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7">
       <c r="A38" t="s">
         <v>63</v>
       </c>
@@ -2259,20 +2259,20 @@
         <v>171</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" s="16" t="s">
+    <row r="40" spans="1:7">
+      <c r="A40" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="B40" s="17"/>
-      <c r="C40" s="17"/>
-      <c r="D40" s="17"/>
-      <c r="E40" s="17"/>
-      <c r="F40" s="17"/>
+      <c r="B40" s="15"/>
+      <c r="C40" s="15"/>
+      <c r="D40" s="15"/>
+      <c r="E40" s="15"/>
+      <c r="F40" s="15"/>
       <c r="G40" s="1" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7">
       <c r="A41" t="s">
         <v>0</v>
       </c>
@@ -2289,7 +2289,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7">
       <c r="A42" t="s">
         <v>66</v>
       </c>
@@ -2306,7 +2306,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7">
       <c r="A43" t="s">
         <v>69</v>
       </c>
@@ -2323,7 +2323,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7">
       <c r="A44" t="s">
         <v>145</v>
       </c>
@@ -2340,7 +2340,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7">
       <c r="A45" t="s">
         <v>148</v>
       </c>
@@ -2357,7 +2357,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7">
       <c r="A46" t="s">
         <v>151</v>
       </c>
@@ -2374,7 +2374,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7">
       <c r="A47" t="s">
         <v>153</v>
       </c>
@@ -2391,7 +2391,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7">
       <c r="A48" t="s">
         <v>182</v>
       </c>
@@ -2408,7 +2408,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7">
       <c r="A49" t="s">
         <v>183</v>
       </c>
@@ -2425,7 +2425,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7">
       <c r="A50" t="s">
         <v>184</v>
       </c>
@@ -2442,7 +2442,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7">
       <c r="A51" t="s">
         <v>88</v>
       </c>
@@ -2459,20 +2459,20 @@
         <v>158</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A52" s="16" t="s">
+    <row r="52" spans="1:7">
+      <c r="A52" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="B52" s="17"/>
-      <c r="C52" s="17"/>
-      <c r="D52" s="17"/>
-      <c r="E52" s="17"/>
-      <c r="F52" s="17"/>
+      <c r="B52" s="15"/>
+      <c r="C52" s="15"/>
+      <c r="D52" s="15"/>
+      <c r="E52" s="15"/>
+      <c r="F52" s="15"/>
       <c r="G52" s="1" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7">
       <c r="A53" t="s">
         <v>0</v>
       </c>
@@ -2489,12 +2489,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7">
       <c r="C54" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7">
       <c r="A55" t="s">
         <v>90</v>
       </c>
@@ -2511,7 +2511,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7">
       <c r="A56" t="s">
         <v>172</v>
       </c>
@@ -2528,7 +2528,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7">
       <c r="A57" t="s">
         <v>173</v>
       </c>
@@ -2545,7 +2545,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7">
       <c r="A58" t="s">
         <v>188</v>
       </c>
@@ -2562,7 +2562,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7">
       <c r="A59" t="s">
         <v>189</v>
       </c>
@@ -2579,7 +2579,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7">
       <c r="A60" t="s">
         <v>190</v>
       </c>
@@ -2596,7 +2596,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7">
       <c r="A61" t="s">
         <v>191</v>
       </c>
@@ -2613,20 +2613,20 @@
         <v>144</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A63" s="16" t="s">
+    <row r="63" spans="1:7">
+      <c r="A63" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="B63" s="17"/>
-      <c r="C63" s="17"/>
-      <c r="D63" s="17"/>
-      <c r="E63" s="17"/>
-      <c r="F63" s="17"/>
+      <c r="B63" s="15"/>
+      <c r="C63" s="15"/>
+      <c r="D63" s="15"/>
+      <c r="E63" s="15"/>
+      <c r="F63" s="15"/>
       <c r="G63" s="1" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7">
       <c r="A64" t="s">
         <v>155</v>
       </c>
@@ -2643,7 +2643,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7">
       <c r="A66" t="s">
         <v>192</v>
       </c>
@@ -2660,7 +2660,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7">
       <c r="A67" t="s">
         <v>193</v>
       </c>
@@ -2677,7 +2677,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7">
       <c r="A68" t="s">
         <v>194</v>
       </c>
@@ -2694,7 +2694,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7">
       <c r="A69" t="s">
         <v>195</v>
       </c>
@@ -2711,7 +2711,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7">
       <c r="A70" t="s">
         <v>196</v>
       </c>
@@ -2728,7 +2728,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7">
       <c r="A71" t="s">
         <v>197</v>
       </c>
@@ -2748,7 +2748,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7">
       <c r="A72" t="s">
         <v>198</v>
       </c>
@@ -2768,7 +2768,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7">
       <c r="A73" t="s">
         <v>199</v>
       </c>
@@ -2788,7 +2788,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7">
       <c r="A74" t="s">
         <v>200</v>
       </c>
@@ -2808,20 +2808,20 @@
         <v>187</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A75" s="16" t="s">
+    <row r="75" spans="1:7">
+      <c r="A75" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="B75" s="17"/>
-      <c r="C75" s="17"/>
-      <c r="D75" s="17"/>
-      <c r="E75" s="17"/>
-      <c r="F75" s="17"/>
+      <c r="B75" s="15"/>
+      <c r="C75" s="15"/>
+      <c r="D75" s="15"/>
+      <c r="E75" s="15"/>
+      <c r="F75" s="15"/>
       <c r="G75" s="1" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7">
       <c r="A76" t="s">
         <v>0</v>
       </c>
@@ -2838,12 +2838,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7">
       <c r="C77" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:7">
       <c r="A78" t="s">
         <v>201</v>
       </c>
@@ -2860,7 +2860,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7">
       <c r="A79" t="s">
         <v>202</v>
       </c>
@@ -2877,7 +2877,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7">
       <c r="A80" t="s">
         <v>203</v>
       </c>
@@ -2894,7 +2894,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:6">
       <c r="A81" t="s">
         <v>204</v>
       </c>
@@ -2911,7 +2911,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:6">
       <c r="A82" t="s">
         <v>205</v>
       </c>
@@ -2928,7 +2928,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:6">
       <c r="A83" t="s">
         <v>206</v>
       </c>
@@ -2945,7 +2945,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:6">
       <c r="A84" t="s">
         <v>207</v>
       </c>
@@ -2962,7 +2962,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:6">
       <c r="A85" t="s">
         <v>208</v>
       </c>
@@ -2979,7 +2979,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:6">
       <c r="A86" t="s">
         <v>209</v>
       </c>
@@ -2996,17 +2996,17 @@
         <v>167</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A87" s="16" t="s">
+    <row r="87" spans="1:6">
+      <c r="A87" s="14" t="s">
         <v>241</v>
       </c>
-      <c r="B87" s="17"/>
-      <c r="C87" s="17"/>
-      <c r="D87" s="17"/>
-      <c r="E87" s="17"/>
-      <c r="F87" s="17"/>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B87" s="15"/>
+      <c r="C87" s="15"/>
+      <c r="D87" s="15"/>
+      <c r="E87" s="15"/>
+      <c r="F87" s="15"/>
+    </row>
+    <row r="88" spans="1:6">
       <c r="A88" s="13" t="s">
         <v>0</v>
       </c>
@@ -3024,7 +3024,7 @@
       </c>
       <c r="F88" s="13"/>
     </row>
-    <row r="89" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:6" ht="43.5">
       <c r="A89" t="s">
         <v>240</v>
       </c>
@@ -3041,7 +3041,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:6" ht="43.5">
       <c r="A90" t="s">
         <v>242</v>
       </c>
@@ -3058,7 +3058,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:6" ht="43.5">
       <c r="A91" t="s">
         <v>243</v>
       </c>
@@ -3075,7 +3075,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:6" ht="43.5">
       <c r="A92" t="s">
         <v>244</v>
       </c>
@@ -3092,7 +3092,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="93" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:6" ht="43.5">
       <c r="A93" t="s">
         <v>245</v>
       </c>
@@ -3109,7 +3109,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="94" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:6" ht="43.5">
       <c r="A94" t="s">
         <v>246</v>
       </c>
@@ -3126,7 +3126,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="95" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:6" ht="43.5">
       <c r="A95" t="s">
         <v>247</v>
       </c>
@@ -3143,7 +3143,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="96" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:6" ht="43.5">
       <c r="A96" t="s">
         <v>248</v>
       </c>
@@ -3160,7 +3160,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="97" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:5" ht="43.5">
       <c r="A97" t="s">
         <v>249</v>
       </c>
@@ -3177,7 +3177,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="98" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:5" ht="43.5">
       <c r="A98" t="s">
         <v>250</v>
       </c>
@@ -3194,7 +3194,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="99" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:5" ht="43.5">
       <c r="A99" t="s">
         <v>251</v>
       </c>
@@ -3211,7 +3211,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="100" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:5" ht="43.5">
       <c r="A100" t="s">
         <v>252</v>
       </c>
@@ -3228,7 +3228,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="101" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:5" ht="43.5">
       <c r="A101" t="s">
         <v>253</v>
       </c>
@@ -3245,7 +3245,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="102" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:5" ht="43.5">
       <c r="A102" t="s">
         <v>254</v>
       </c>
@@ -3262,7 +3262,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="103" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:5" ht="58">
       <c r="A103" t="s">
         <v>255</v>
       </c>
@@ -3279,7 +3279,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="104" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:5" ht="58">
       <c r="A104" t="s">
         <v>270</v>
       </c>
@@ -3296,7 +3296,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="105" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:5" ht="58">
       <c r="A105" t="s">
         <v>271</v>
       </c>
@@ -3313,7 +3313,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="106" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:5" ht="58">
       <c r="A106" t="s">
         <v>288</v>
       </c>
@@ -3332,12 +3332,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A87:F87"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:F3"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="A40:F40"/>
     <mergeCell ref="A52:F52"/>
@@ -3345,6 +3339,12 @@
     <mergeCell ref="A75:F75"/>
     <mergeCell ref="A15:F15"/>
     <mergeCell ref="A27:F27"/>
+    <mergeCell ref="A87:F87"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>